<commit_message>
created backbone of invite/accept system, run a basic test and data is working. I need to extract object creation to a different class. Clientside validation will be done by said new class
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301 - individual project\Planning Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C1F8BCD-3CF7-4106-9D50-682F2D90466B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB8EB1F-DD85-4E81-9EFE-B08E41338B26}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
   <si>
     <t>Task</t>
   </si>
@@ -231,6 +231,21 @@
   </si>
   <si>
     <t>2. Requirement</t>
+  </si>
+  <si>
+    <t>Release Use cases</t>
+  </si>
+  <si>
+    <t>Release Wireframes</t>
+  </si>
+  <si>
+    <t>3. meeting</t>
+  </si>
+  <si>
+    <t>Use Cases</t>
+  </si>
+  <si>
+    <t>Wireframes/Flow</t>
   </si>
 </sst>
 </file>
@@ -351,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -564,6 +579,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -628,7 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -762,27 +788,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,9 +796,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
@@ -810,6 +812,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -968,42 +1003,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$14:$O$14</c:f>
+              <c:f>'Sprint Backlog 1'!$E$16:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>33.5</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.15</c:v>
+                  <c:v>37.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.799999999999997</c:v>
+                  <c:v>33.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.449999999999996</c:v>
+                  <c:v>29.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.099999999999994</c:v>
+                  <c:v>24.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.749999999999993</c:v>
+                  <c:v>20.750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.399999999999993</c:v>
+                  <c:v>16.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.049999999999994</c:v>
+                  <c:v>12.450000000000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.699999999999994</c:v>
+                  <c:v>8.3000000000000078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.3499999999999939</c:v>
+                  <c:v>4.1500000000000075</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-6.2172489379008766E-15</c:v>
+                  <c:v>7.1054273576010019E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1067,42 +1102,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$15:$O$15</c:f>
+              <c:f>'Sprint Backlog 1'!$E$17:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>33.5</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1302,42 +1337,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$14:$O$14</c:f>
+              <c:f>'Sprint Backlog 1'!$E$16:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>33.5</c:v>
+                  <c:v>41.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.15</c:v>
+                  <c:v>37.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.799999999999997</c:v>
+                  <c:v>33.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.449999999999996</c:v>
+                  <c:v>29.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.099999999999994</c:v>
+                  <c:v>24.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.749999999999993</c:v>
+                  <c:v>20.750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.399999999999993</c:v>
+                  <c:v>16.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.049999999999994</c:v>
+                  <c:v>12.450000000000008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.699999999999994</c:v>
+                  <c:v>8.3000000000000078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.3499999999999939</c:v>
+                  <c:v>4.1500000000000075</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-6.2172489379008766E-15</c:v>
+                  <c:v>7.1054273576010019E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,13 +1595,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>467784</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>80435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>245533</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2343,10 +2378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:U15"/>
+  <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2367,37 +2402,37 @@
     <col min="16" max="16" width="5.875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-    </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="51" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-    </row>
-    <row r="3" spans="2:21" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+    </row>
+    <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
@@ -2444,15 +2479,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="61" t="s">
+    <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="54" t="s">
         <v>57</v>
       </c>
       <c r="D4" s="31"/>
-      <c r="E4" s="58">
+      <c r="E4" s="51">
         <v>4</v>
       </c>
       <c r="F4" s="4">
@@ -2490,11 +2525,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="61"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="60"/>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="66"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="4">
         <v>0</v>
       </c>
@@ -2526,17 +2561,17 @@
         <v>0</v>
       </c>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P13" si="0">SUM(F5:O5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="61"/>
-      <c r="C6" s="64" t="s">
+        <f t="shared" ref="P5:P15" si="0">SUM(F5:O5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="66"/>
+      <c r="C6" s="56" t="s">
         <v>62</v>
       </c>
       <c r="D6" s="31"/>
-      <c r="E6" s="60">
+      <c r="E6" s="53">
         <v>0.5</v>
       </c>
       <c r="F6" s="4">
@@ -2574,11 +2609,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="61"/>
-      <c r="C7" s="63"/>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="66"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="31"/>
-      <c r="E7" s="59"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="4">
         <v>0</v>
       </c>
@@ -2614,19 +2649,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="55" t="s">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="59" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="31"/>
-      <c r="E8" s="60">
+      <c r="E8" s="53">
         <v>8</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2657,20 +2692,20 @@
       </c>
       <c r="P8" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="57"/>
-      <c r="C9" s="64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="65"/>
+      <c r="C9" s="56" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="31"/>
-      <c r="E9" s="59">
+      <c r="E9" s="52">
         <v>4</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -2701,20 +2736,20 @@
       </c>
       <c r="P9" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
-      <c r="C10" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="65"/>
+      <c r="C10" s="54" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="31"/>
-      <c r="E10" s="59">
+      <c r="E10" s="52">
         <v>8</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -2745,16 +2780,16 @@
       </c>
       <c r="P10" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="56"/>
-      <c r="C11" s="64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="67"/>
+      <c r="C11" s="56" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="59">
+      <c r="E11" s="52">
         <v>8</v>
       </c>
       <c r="F11" s="4">
@@ -2792,22 +2827,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="55" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="62" t="s">
-        <v>63</v>
+      <c r="C12" s="56" t="s">
+        <v>69</v>
       </c>
       <c r="D12" s="31"/>
-      <c r="E12" s="60">
-        <v>0.5</v>
+      <c r="E12" s="70">
+        <v>4</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
@@ -2835,172 +2870,273 @@
       </c>
       <c r="P12" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="57"/>
-      <c r="C13" s="62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="67"/>
+      <c r="C13" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="70">
+        <v>4</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="20">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="20">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="65"/>
+      <c r="C15" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="59">
+      <c r="D15" s="31"/>
+      <c r="E15" s="52">
         <v>0.5</v>
       </c>
-      <c r="F13" s="4">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="20">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="54" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="23">
-        <f>SUM(E4:E13)</f>
-        <v>33.5</v>
-      </c>
-      <c r="F14" s="17">
-        <f t="shared" ref="F14:O14" si="1">E14-$E$14/10</f>
-        <v>30.15</v>
-      </c>
-      <c r="G14" s="17">
+      <c r="C16" s="63"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="23">
+        <f>SUM(E4:E15)</f>
+        <v>41.5</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" ref="F16:O16" si="1">E16-$E$16/10</f>
+        <v>37.35</v>
+      </c>
+      <c r="G16" s="17">
         <f t="shared" si="1"/>
-        <v>26.799999999999997</v>
-      </c>
-      <c r="H14" s="17">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="H16" s="17">
         <f t="shared" si="1"/>
-        <v>23.449999999999996</v>
-      </c>
-      <c r="I14" s="17">
+        <v>29.050000000000004</v>
+      </c>
+      <c r="I16" s="17">
         <f t="shared" si="1"/>
-        <v>20.099999999999994</v>
-      </c>
-      <c r="J14" s="18">
+        <v>24.900000000000006</v>
+      </c>
+      <c r="J16" s="18">
         <f t="shared" si="1"/>
-        <v>16.749999999999993</v>
-      </c>
-      <c r="K14" s="17">
+        <v>20.750000000000007</v>
+      </c>
+      <c r="K16" s="17">
         <f t="shared" si="1"/>
-        <v>13.399999999999993</v>
-      </c>
-      <c r="L14" s="17">
+        <v>16.600000000000009</v>
+      </c>
+      <c r="L16" s="17">
         <f t="shared" si="1"/>
-        <v>10.049999999999994</v>
-      </c>
-      <c r="M14" s="17">
+        <v>12.450000000000008</v>
+      </c>
+      <c r="M16" s="17">
         <f t="shared" si="1"/>
-        <v>6.699999999999994</v>
-      </c>
-      <c r="N14" s="17">
+        <v>8.3000000000000078</v>
+      </c>
+      <c r="N16" s="17">
         <f t="shared" si="1"/>
-        <v>3.3499999999999939</v>
-      </c>
-      <c r="O14" s="18">
+        <v>4.1500000000000075</v>
+      </c>
+      <c r="O16" s="18">
         <f t="shared" si="1"/>
-        <v>-6.2172489379008766E-15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="54" t="s">
+        <v>7.1054273576010019E-15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="10">
-        <f>SUM(E4:E13)</f>
-        <v>33.5</v>
-      </c>
-      <c r="F15" s="6">
-        <f>E15-(SUM(F4:F13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="G15" s="6">
-        <f>F15-(SUM(G4:G13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="H15" s="6">
-        <f>G15-(SUM(H4:H13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="I15" s="6">
-        <f>H15-(SUM(I4:I13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="J15" s="21">
-        <f>I15-(SUM(J4:J13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="K15" s="6">
-        <f>J15-(SUM(K4:K13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="L15" s="6">
-        <f>K15-(SUM(L4:L13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="M15" s="6">
-        <f>L15-(SUM(M4:M13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="N15" s="6">
-        <f>M15-(SUM(N4:N13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="O15" s="7">
-        <f>N15-(SUM(O4:O13))</f>
-        <v>33.5</v>
-      </c>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="10">
+        <f>SUM(E4:E15)</f>
+        <v>41.5</v>
+      </c>
+      <c r="F17" s="6">
+        <f>E17-(SUM(F4:F15))</f>
+        <v>31.5</v>
+      </c>
+      <c r="G17" s="6">
+        <f>F17-(SUM(G4:G15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="H17" s="6">
+        <f>G17-(SUM(H4:H15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="I17" s="6">
+        <f>H17-(SUM(I4:I15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="J17" s="21">
+        <f>I17-(SUM(J4:J15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="K17" s="6">
+        <f>J17-(SUM(K4:K15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="L17" s="6">
+        <f>K17-(SUM(L4:L15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="M17" s="6">
+        <f>L17-(SUM(M4:M15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="N17" s="6">
+        <f>M17-(SUM(N4:N15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="O17" s="7">
+        <f>N17-(SUM(O4:O15))</f>
+        <v>27.5</v>
+      </c>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C22" s="69" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3012,7 +3148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:W18"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -3037,38 +3173,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="51" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3124,7 +3260,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="64" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -3178,7 +3314,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -3230,7 +3366,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="64" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -3276,7 +3412,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="57"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -3320,7 +3456,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="57"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -3364,7 +3500,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="57"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -3408,7 +3544,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -3452,7 +3588,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -3496,7 +3632,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="57"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -3540,7 +3676,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="57"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -3584,7 +3720,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="57"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -3628,7 +3764,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="57"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -3672,7 +3808,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="56"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -3716,11 +3852,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -3769,11 +3905,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -3829,14 +3965,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
created generalised class to create document data. Added QR code generation.
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31279384-8FFA-4F6F-A648-B7EB453CC676}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5C5824-8D17-473D-A6DF-026CD6F56807}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,6 +206,9 @@
     <t>Will delay until sprint 7 probably.</t>
   </si>
   <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
     <t>User Login</t>
   </si>
   <si>
@@ -230,22 +233,19 @@
     <t>2. Requirement</t>
   </si>
   <si>
-    <t>Release Use cases</t>
-  </si>
-  <si>
-    <t>Release Wireframes</t>
-  </si>
-  <si>
-    <t>3. meeting</t>
-  </si>
-  <si>
-    <t>Use Cases</t>
-  </si>
-  <si>
-    <t>Wireframes/Flow</t>
-  </si>
-  <si>
-    <t>Reflection</t>
+    <t>Use cases/flow diagrams</t>
+  </si>
+  <si>
+    <t>Team Invite QR Reading</t>
+  </si>
+  <si>
+    <t>Team Invite QR Generation</t>
+  </si>
+  <si>
+    <t>Team Modification</t>
+  </si>
+  <si>
+    <t>Team Display</t>
   </si>
 </sst>
 </file>
@@ -352,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,8 +365,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -581,17 +587,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="6" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -813,6 +808,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,14 +838,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1003,42 +998,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$16:$O$16</c:f>
+              <c:f>'Sprint Backlog 1'!$E$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>41.5</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.35</c:v>
+                  <c:v>42.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.200000000000003</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.050000000000004</c:v>
+                  <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.900000000000006</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.750000000000007</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.600000000000009</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.450000000000008</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.3000000000000078</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1500000000000075</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.1054273576010019E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1102,42 +1097,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$17:$O$17</c:f>
+              <c:f>'Sprint Backlog 1'!$E$19:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>41.5</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1337,42 +1332,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$16:$O$16</c:f>
+              <c:f>'Sprint Backlog 1'!$E$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>41.5</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.35</c:v>
+                  <c:v>42.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.200000000000003</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.050000000000004</c:v>
+                  <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.900000000000006</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.750000000000007</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.600000000000009</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.450000000000008</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.3000000000000078</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1500000000000075</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.1054273576010019E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1595,13 +1590,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>467784</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>80435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>245533</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2378,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:U22"/>
+  <dimension ref="B1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2403,34 +2398,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="60" t="s">
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -2480,10 +2475,12 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="54" t="s">
+        <v>57</v>
+      </c>
       <c r="D4" s="31"/>
       <c r="E4" s="51">
         <v>4</v>
@@ -2495,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
@@ -2520,30 +2517,32 @@
       </c>
       <c r="P4" s="23">
         <f>SUM(F4:O4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="66"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="68"/>
       <c r="C5" s="57" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D5" s="58"/>
-      <c r="E5" s="53"/>
+      <c r="E5" s="53">
+        <v>4</v>
+      </c>
       <c r="F5" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
       </c>
       <c r="J5" s="20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="4">
         <v>0</v>
@@ -2561,14 +2560,14 @@
         <v>0</v>
       </c>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P15" si="0">SUM(F5:O5)</f>
-        <v>1</v>
+        <f t="shared" ref="P5:P17" si="0">SUM(F5:O5)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="66"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="56" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="53">
@@ -2610,7 +2609,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="66"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -2649,34 +2648,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>60</v>
+    <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>67</v>
       </c>
       <c r="D8" s="31"/>
-      <c r="E8" s="53">
-        <v>8</v>
+      <c r="E8" s="60">
+        <v>2</v>
       </c>
       <c r="F8" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <v>1</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="20">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <v>0</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
@@ -2692,35 +2691,35 @@
       </c>
       <c r="P8" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="65"/>
-      <c r="C9" s="56" t="s">
-        <v>57</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="67"/>
+      <c r="C9" s="57" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="31"/>
-      <c r="E9" s="52">
-        <v>4</v>
+      <c r="E9" s="60">
+        <v>2</v>
       </c>
       <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
         <v>2</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="20">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
@@ -2740,23 +2739,23 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="65"/>
-      <c r="C10" s="54" t="s">
-        <v>58</v>
+      <c r="B10" s="67"/>
+      <c r="C10" s="59" t="s">
+        <v>61</v>
       </c>
       <c r="D10" s="31"/>
-      <c r="E10" s="52">
+      <c r="E10" s="53">
         <v>8</v>
       </c>
       <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
         <v>4</v>
       </c>
-      <c r="G10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
       <c r="I10" s="4">
         <v>0</v>
       </c>
@@ -2778,25 +2777,25 @@
       <c r="O10" s="4">
         <v>0</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="70">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="67"/>
       <c r="C11" s="56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="52">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -2824,25 +2823,23 @@
       </c>
       <c r="P11" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>68</v>
+      <c r="B12" s="67"/>
+      <c r="C12" s="54" t="s">
+        <v>59</v>
       </c>
       <c r="D12" s="31"/>
-      <c r="E12" s="70">
+      <c r="E12" s="52">
+        <v>8</v>
+      </c>
+      <c r="F12" s="4">
         <v>4</v>
       </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
@@ -2870,69 +2867,65 @@
       </c>
       <c r="P12" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="67"/>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="52">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="20">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" ref="P13:P14" si="1">SUM(F13:O13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="67"/>
+      <c r="C14" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="70">
+      <c r="D14" s="31"/>
+      <c r="E14" s="52">
         <v>4</v>
       </c>
-      <c r="F13" s="4">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="53">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="F14" s="4"/>
       <c r="G14" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H14" s="4">
         <v>0</v>
@@ -2959,184 +2952,263 @@
         <v>0</v>
       </c>
       <c r="P14" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="65"/>
-      <c r="C15" s="54" t="s">
-        <v>63</v>
+      <c r="B15" s="69"/>
+      <c r="C15" s="56" t="s">
+        <v>60</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="52">
+        <v>8</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>4</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="20">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>4</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="53">
         <v>0.5</v>
       </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="20">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="4">
-        <v>0</v>
-      </c>
-      <c r="P15" s="10">
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="63" t="s">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="67"/>
+      <c r="C17" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="23">
-        <f>SUM(E4:E15)</f>
-        <v>41.5</v>
-      </c>
-      <c r="F16" s="17">
-        <f t="shared" ref="F16:O16" si="1">E16-$E$16/10</f>
-        <v>37.35</v>
-      </c>
-      <c r="G16" s="17">
-        <f t="shared" si="1"/>
-        <v>33.200000000000003</v>
-      </c>
-      <c r="H16" s="17">
-        <f t="shared" si="1"/>
-        <v>29.050000000000004</v>
-      </c>
-      <c r="I16" s="17">
-        <f t="shared" si="1"/>
-        <v>24.900000000000006</v>
-      </c>
-      <c r="J16" s="18">
-        <f t="shared" si="1"/>
-        <v>20.750000000000007</v>
-      </c>
-      <c r="K16" s="17">
-        <f t="shared" si="1"/>
-        <v>16.600000000000009</v>
-      </c>
-      <c r="L16" s="17">
-        <f t="shared" si="1"/>
-        <v>12.450000000000008</v>
-      </c>
-      <c r="M16" s="17">
-        <f t="shared" si="1"/>
-        <v>8.3000000000000078</v>
-      </c>
-      <c r="N16" s="17">
-        <f t="shared" si="1"/>
-        <v>4.1500000000000075</v>
-      </c>
-      <c r="O16" s="18">
-        <f t="shared" si="1"/>
-        <v>7.1054273576010019E-15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="63" t="s">
+      <c r="C18" s="65"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="23">
+        <f>SUM(E4:E17)</f>
+        <v>47.5</v>
+      </c>
+      <c r="F18" s="17">
+        <f t="shared" ref="F18:O18" si="2">E18-$E$18/10</f>
+        <v>42.75</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="H18" s="17">
+        <f t="shared" si="2"/>
+        <v>33.25</v>
+      </c>
+      <c r="I18" s="17">
+        <f t="shared" si="2"/>
+        <v>28.5</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="2"/>
+        <v>23.75</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="L18" s="17">
+        <f t="shared" si="2"/>
+        <v>14.25</v>
+      </c>
+      <c r="M18" s="17">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+      <c r="N18" s="17">
+        <f t="shared" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="O18" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="10">
-        <f>SUM(E4:E15)</f>
-        <v>41.5</v>
-      </c>
-      <c r="F17" s="6">
-        <f>E17-(SUM(F4:F15))</f>
-        <v>30</v>
-      </c>
-      <c r="G17" s="6">
-        <f>F17-(SUM(G4:G15))</f>
-        <v>22</v>
-      </c>
-      <c r="H17" s="6">
-        <f>G17-(SUM(H4:H15))</f>
-        <v>22</v>
-      </c>
-      <c r="I17" s="6">
-        <f>H17-(SUM(I4:I15))</f>
-        <v>22</v>
-      </c>
-      <c r="J17" s="21">
-        <f>I17-(SUM(J4:J15))</f>
-        <v>22</v>
-      </c>
-      <c r="K17" s="6">
-        <f>J17-(SUM(K4:K15))</f>
-        <v>22</v>
-      </c>
-      <c r="L17" s="6">
-        <f>K17-(SUM(L4:L15))</f>
-        <v>22</v>
-      </c>
-      <c r="M17" s="6">
-        <f>L17-(SUM(M4:M15))</f>
-        <v>22</v>
-      </c>
-      <c r="N17" s="6">
-        <f>M17-(SUM(N4:N15))</f>
-        <v>22</v>
-      </c>
-      <c r="O17" s="7">
-        <f>N17-(SUM(O4:O15))</f>
-        <v>22</v>
-      </c>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C21" s="68" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C22" s="69" t="s">
-        <v>66</v>
-      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="10">
+        <f>SUM(E4:E17)</f>
+        <v>47.5</v>
+      </c>
+      <c r="F19" s="6">
+        <f>E19-(SUM(F4:F17))</f>
+        <v>36</v>
+      </c>
+      <c r="G19" s="6">
+        <f>F19-(SUM(G4:G17))</f>
+        <v>35.5</v>
+      </c>
+      <c r="H19" s="6">
+        <f>G19-(SUM(H4:H17))</f>
+        <v>21.5</v>
+      </c>
+      <c r="I19" s="6">
+        <f>H19-(SUM(I4:I17))</f>
+        <v>21.5</v>
+      </c>
+      <c r="J19" s="21">
+        <f>I19-(SUM(J4:J17))</f>
+        <v>18.5</v>
+      </c>
+      <c r="K19" s="6">
+        <f>J19-(SUM(K4:K17))</f>
+        <v>11.5</v>
+      </c>
+      <c r="L19" s="6">
+        <f>K19-(SUM(L4:L17))</f>
+        <v>11.5</v>
+      </c>
+      <c r="M19" s="6">
+        <f>L19-(SUM(M4:M17))</f>
+        <v>11.5</v>
+      </c>
+      <c r="N19" s="6">
+        <f>M19-(SUM(N4:N17))</f>
+        <v>11.5</v>
+      </c>
+      <c r="O19" s="7">
+        <f>N19-(SUM(O4:O17))</f>
+        <v>11.5</v>
+      </c>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B8:B15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3148,7 +3220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:W18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -3173,38 +3245,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="60" t="s">
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3260,7 +3332,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="66" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -3314,7 +3386,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="67"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -3366,7 +3438,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="66" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -3412,7 +3484,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="65"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -3456,7 +3528,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="65"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -3500,7 +3572,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="65"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -3544,7 +3616,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="65"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -3588,7 +3660,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="65"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -3632,7 +3704,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="65"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -3676,7 +3748,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="65"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -3720,7 +3792,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="65"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -3764,7 +3836,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="65"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -3808,7 +3880,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="67"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -3852,11 +3924,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -3905,11 +3977,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -3965,14 +4037,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
small cleanup on code, filed in admin stuff. The description for today is a bit thin, will elaborate tomorrow
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DCCADF-10A9-4936-9F76-2AEB634D2FEF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962077EC-71C6-4214-B8F9-12B81B508370}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="22275" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="600" windowWidth="22275" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -1126,13 +1126,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2375,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" s="4">
         <v>0</v>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="P10" s="62">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -2943,7 +2943,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" s="4">
         <v>0</v>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="P14" s="9">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -2987,7 +2987,7 @@
         <v>2</v>
       </c>
       <c r="M15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15" s="4">
         <v>0</v>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="P15" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -3181,15 +3181,15 @@
       </c>
       <c r="M19" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="N19" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="O19" s="7">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="2"/>
@@ -4037,14 +4037,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
created a new sprint with broken down version of tasks, created a new list of tasks. Added task navigation to the site. Upgraded form to be able to create tasks as well as teams.
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962077EC-71C6-4214-B8F9-12B81B508370}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB0E32B-3FEB-40FE-976A-31AAE2391D25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="600" windowWidth="22275" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
     <sheet name="Sprint Backlog 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sprint Backlog 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sprint Backlog 1 (2)" sheetId="6" r:id="rId3"/>
+    <sheet name="Sprint Backlog 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
   <si>
     <t>Task</t>
   </si>
@@ -119,9 +120,6 @@
     <t>3. user story</t>
   </si>
   <si>
-    <t>date of sprint</t>
-  </si>
-  <si>
     <t>How long (hours)</t>
   </si>
   <si>
@@ -246,6 +244,66 @@
   </si>
   <si>
     <t>Team Display</t>
+  </si>
+  <si>
+    <t>sprint planning</t>
+  </si>
+  <si>
+    <t>Task Viewing - Navigation</t>
+  </si>
+  <si>
+    <t>Task Viewing - item render</t>
+  </si>
+  <si>
+    <t>Task Viewing - list render</t>
+  </si>
+  <si>
+    <t>Task Viewing - shared update</t>
+  </si>
+  <si>
+    <t>UML Diagrams - Task creation, render, invite</t>
+  </si>
+  <si>
+    <t>UML Diagrams - Team creation, render, invite</t>
+  </si>
+  <si>
+    <t>Client-side validation -User</t>
+  </si>
+  <si>
+    <t>Task - wireframes</t>
+  </si>
+  <si>
+    <t>Task - flow diagrams</t>
+  </si>
+  <si>
+    <t>Supervisor Meeting x2</t>
+  </si>
+  <si>
+    <t>Card Render Update</t>
+  </si>
+  <si>
+    <t>Unit Testing</t>
+  </si>
+  <si>
+    <t>Jquery QR reader POC</t>
+  </si>
+  <si>
+    <t>Affordance UX based css</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Deliverable</t>
+  </si>
+  <si>
+    <t>04/11/19-15/11/19</t>
+  </si>
+  <si>
+    <t>18/11/19-29/11/19</t>
   </si>
 </sst>
 </file>
@@ -352,7 +410,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,8 +429,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -587,6 +657,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="6" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -649,7 +769,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -817,6 +937,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -840,6 +963,39 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1251,6 +1407,340 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16282253282832151"/>
+          <c:y val="1.8470584658792262E-2"/>
+          <c:w val="0.71469100453352397"/>
+          <c:h val="0.79831147760594201"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 1 (2)'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 1 (2)'!$E$19:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.600000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.800000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4000000000000061</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2172489379008766E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6760-494C-95FC-DD95C97B6953}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 1 (2)'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 1 (2)'!$E$20:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6760-494C-95FC-DD95C97B6953}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="132299304"/>
+        <c:axId val="132299696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="132299304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DAYS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="132299696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>HOURS EFFORT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1626,6 +2116,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>475111</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>131724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>252860</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>121138</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C1CFF79-57E4-49CC-A50D-6AF84C98015B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2009,30 +2542,30 @@
     <row r="1" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" s="1" customFormat="1" ht="42.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="G2" s="39" t="s">
         <v>30</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>34</v>
       </c>
       <c r="D3" s="43">
         <v>1</v>
@@ -2041,18 +2574,18 @@
         <v>12</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="47">
         <v>2</v>
@@ -2061,18 +2594,18 @@
         <v>16</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="47">
         <v>2</v>
@@ -2081,18 +2614,18 @@
         <v>4</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="47">
         <v>3</v>
@@ -2101,18 +2634,18 @@
         <v>32</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="47">
         <v>4</v>
@@ -2121,18 +2654,18 @@
         <v>16</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" s="46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="47">
         <v>4</v>
@@ -2141,18 +2674,18 @@
         <v>16</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="46" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="46" t="s">
-        <v>54</v>
       </c>
       <c r="D9" s="47">
         <v>5</v>
@@ -2161,18 +2694,18 @@
         <v>32</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="50">
         <v>6</v>
@@ -2181,18 +2714,18 @@
         <v>16</v>
       </c>
       <c r="F10" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="47">
         <v>6</v>
@@ -2201,10 +2734,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="46" t="s">
         <v>41</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="21" x14ac:dyDescent="0.35">
@@ -2375,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2398,34 +2931,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64" t="s">
+      <c r="C2" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="63" t="s">
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -2475,11 +3008,11 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="70" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="51">
@@ -2521,9 +3054,9 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="53">
@@ -2565,9 +3098,9 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="53">
@@ -2609,7 +3142,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -2649,11 +3182,11 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="67" t="s">
-        <v>65</v>
+      <c r="B8" s="68" t="s">
+        <v>64</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="60">
@@ -2695,9 +3228,9 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="60">
@@ -2739,9 +3272,9 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="53">
@@ -2783,9 +3316,9 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="52">
@@ -2827,9 +3360,9 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="52">
@@ -2865,15 +3398,15 @@
       <c r="O12" s="4">
         <v>0</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="81">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="52">
@@ -2915,9 +3448,9 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="52">
@@ -2951,15 +3484,15 @@
       <c r="O14" s="4">
         <v>0</v>
       </c>
-      <c r="P14" s="9">
+      <c r="P14" s="82">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="70"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="52">
@@ -2995,17 +3528,17 @@
       <c r="O15" s="4">
         <v>0</v>
       </c>
-      <c r="P15" s="9">
+      <c r="P15" s="82">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="68" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="53">
@@ -3047,9 +3580,9 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="52">
@@ -3091,10 +3624,10 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="32"/>
       <c r="E18" s="23">
         <f>SUM(E4:E17)</f>
@@ -3142,10 +3675,10 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="66"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="33"/>
       <c r="E19" s="10">
         <f>SUM(E4:E17)</f>
@@ -3217,11 +3750,655 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E71DFC-EBA7-4F4A-8776-6F171A9158CA}">
+  <dimension ref="B1:U35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="7" width="7.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="7" style="5" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7.625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="5.875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+    </row>
+    <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="51">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="23">
+        <f>SUM(F4:O4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53">
+        <v>4</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="9">
+        <f t="shared" ref="P5:P18" si="0">SUM(F5:O5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="69"/>
+      <c r="C6" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="53">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="69"/>
+      <c r="C7" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="52">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="71"/>
+      <c r="C8" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="60">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="60">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="70"/>
+      <c r="C10" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="53">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="70"/>
+      <c r="C11" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="52">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="70"/>
+      <c r="C12" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="52">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="70"/>
+      <c r="C13" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="52">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="63"/>
+      <c r="C14" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="52">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="63"/>
+      <c r="C15" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="52">
+        <v>4</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="63"/>
+      <c r="C16" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="53">
+        <v>4</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="63"/>
+      <c r="C17" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="53">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="9"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="63"/>
+      <c r="C18" s="79" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="52">
+        <v>4</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="67"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="23">
+        <f>SUM(E4:E18)</f>
+        <v>34</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" ref="F19:O19" si="1">E19-$E$19/10</f>
+        <v>30.6</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="1"/>
+        <v>27.200000000000003</v>
+      </c>
+      <c r="H19" s="17">
+        <f t="shared" si="1"/>
+        <v>23.800000000000004</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="1"/>
+        <v>20.400000000000006</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="1"/>
+        <v>17.000000000000007</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="1"/>
+        <v>13.600000000000007</v>
+      </c>
+      <c r="L19" s="17">
+        <f t="shared" si="1"/>
+        <v>10.200000000000006</v>
+      </c>
+      <c r="M19" s="17">
+        <f t="shared" si="1"/>
+        <v>6.800000000000006</v>
+      </c>
+      <c r="N19" s="17">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000061</v>
+      </c>
+      <c r="O19" s="18">
+        <f t="shared" si="1"/>
+        <v>6.2172489379008766E-15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="67"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="10">
+        <f>SUM(E4:E18)</f>
+        <v>34</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" ref="F20:O20" si="2">E20-(SUM(F4:F18))</f>
+        <v>27</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="J20" s="21">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="M20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O20" s="7">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R21" s="72"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R22" s="73"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R23" s="72"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R24" s="73"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R25" s="72"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R26" s="73"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R27" s="72"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R28" s="73"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R29" s="72"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R30" s="73"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R31" s="72"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R32" s="73"/>
+    </row>
+    <row r="33" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R33" s="72"/>
+    </row>
+    <row r="34" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R34" s="73"/>
+    </row>
+    <row r="35" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R35" s="72"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:W18"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="B2:R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3245,38 +4422,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="63" t="s">
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3332,7 +4509,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="68" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -3386,7 +4563,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -3438,7 +4615,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -3484,7 +4661,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="68"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -3528,7 +4705,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -3572,7 +4749,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -3616,7 +4793,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="68"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -3660,7 +4837,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="68"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -3704,7 +4881,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -3748,7 +4925,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="68"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -3792,7 +4969,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="68"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -3836,7 +5013,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="68"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -3880,7 +5057,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="70"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -3924,11 +5101,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -3977,11 +5154,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -4037,14 +5214,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
pushing up some libs
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB0E32B-3FEB-40FE-976A-31AAE2391D25}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2A110B-947C-4DF1-9F69-30A46EA6F83C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>Task</t>
   </si>
@@ -276,12 +276,6 @@
     <t>Task - flow diagrams</t>
   </si>
   <si>
-    <t>Supervisor Meeting x2</t>
-  </si>
-  <si>
-    <t>Card Render Update</t>
-  </si>
-  <si>
     <t>Unit Testing</t>
   </si>
   <si>
@@ -304,6 +298,12 @@
   </si>
   <si>
     <t>18/11/19-29/11/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisor Meeting </t>
+  </si>
+  <si>
+    <t>Task Creation</t>
   </si>
 </sst>
 </file>
@@ -769,7 +769,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -940,6 +940,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -963,39 +999,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1488,7 +1491,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1 (2)'!$E$19:$O$19</c:f>
+              <c:f>'Sprint Backlog 1 (2)'!$E$20:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1587,7 +1590,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1 (2)'!$E$20:$O$20</c:f>
+              <c:f>'Sprint Backlog 1 (2)'!$E$21:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1598,31 +1601,31 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2121,13 +2124,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>475111</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>131724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>252860</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2931,34 +2934,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65" t="s">
+      <c r="C2" s="77" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="64" t="s">
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3008,7 +3011,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="54" t="s">
@@ -3054,7 +3057,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="57" t="s">
         <v>65</v>
       </c>
@@ -3098,7 +3101,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="56" t="s">
         <v>61</v>
       </c>
@@ -3142,7 +3145,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="70"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -3182,7 +3185,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="80" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="61" t="s">
@@ -3228,7 +3231,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="69"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="57" t="s">
         <v>67</v>
       </c>
@@ -3272,7 +3275,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="69"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="59" t="s">
         <v>60</v>
       </c>
@@ -3316,7 +3319,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="69"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="56" t="s">
         <v>57</v>
       </c>
@@ -3360,7 +3363,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="54" t="s">
         <v>58</v>
       </c>
@@ -3398,13 +3401,13 @@
       <c r="O12" s="4">
         <v>0</v>
       </c>
-      <c r="P12" s="81">
+      <c r="P12" s="74">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="54" t="s">
         <v>69</v>
       </c>
@@ -3448,7 +3451,7 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="54" t="s">
         <v>68</v>
       </c>
@@ -3484,13 +3487,13 @@
       <c r="O14" s="4">
         <v>0</v>
       </c>
-      <c r="P14" s="82">
+      <c r="P14" s="75">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="71"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="56" t="s">
         <v>59</v>
       </c>
@@ -3528,13 +3531,13 @@
       <c r="O15" s="4">
         <v>0</v>
       </c>
-      <c r="P15" s="82">
+      <c r="P15" s="75">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="80" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="54" t="s">
@@ -3580,7 +3583,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="54" t="s">
         <v>63</v>
       </c>
@@ -3624,10 +3627,10 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="32"/>
       <c r="E18" s="23">
         <f>SUM(E4:E17)</f>
@@ -3675,10 +3678,10 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="67"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="33"/>
       <c r="E19" s="10">
         <f>SUM(E4:E17)</f>
@@ -3751,10 +3754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E71DFC-EBA7-4F4A-8776-6F171A9158CA}">
-  <dimension ref="B1:U35"/>
+  <dimension ref="B1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3776,34 +3779,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="65" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65" t="s">
+      <c r="C2" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="64" t="s">
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3854,9 +3857,9 @@
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="71" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="31"/>
@@ -3881,10 +3884,10 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="80" t="s">
+      <c r="B5" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="73" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="58"/>
@@ -3904,13 +3907,13 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P18" si="0">SUM(F5:O5)</f>
+        <f t="shared" ref="P5:P19" si="0">SUM(F5:O5)</f>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
-      <c r="C6" s="72" t="s">
+      <c r="B6" s="81"/>
+      <c r="C6" s="65" t="s">
         <v>72</v>
       </c>
       <c r="D6" s="31"/>
@@ -3919,7 +3922,9 @@
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="20"/>
       <c r="K6" s="4"/>
@@ -3929,12 +3934,12 @@
       <c r="O6" s="4"/>
       <c r="P6" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="81"/>
+      <c r="C7" s="66" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="31"/>
@@ -3945,7 +3950,9 @@
         <v>1</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="20"/>
       <c r="K7" s="4"/>
@@ -3955,12 +3962,12 @@
       <c r="O7" s="4"/>
       <c r="P7" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="71"/>
-      <c r="C8" s="72" t="s">
+      <c r="B8" s="83"/>
+      <c r="C8" s="65" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="31"/>
@@ -3985,10 +3992,10 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="74" t="s">
+      <c r="B9" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="67" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="31"/>
@@ -4011,8 +4018,8 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="70"/>
-      <c r="C10" s="75" t="s">
+      <c r="B10" s="82"/>
+      <c r="C10" s="68" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="31"/>
@@ -4035,8 +4042,8 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="70"/>
-      <c r="C11" s="76" t="s">
+      <c r="B11" s="82"/>
+      <c r="C11" s="69" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="31"/>
@@ -4059,8 +4066,8 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="70"/>
-      <c r="C12" s="75" t="s">
+      <c r="B12" s="82"/>
+      <c r="C12" s="68" t="s">
         <v>78</v>
       </c>
       <c r="D12" s="31"/>
@@ -4068,7 +4075,9 @@
         <v>1</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="20"/>
@@ -4079,12 +4088,12 @@
       <c r="O12" s="4"/>
       <c r="P12" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="70"/>
-      <c r="C13" s="77" t="s">
+      <c r="B13" s="82"/>
+      <c r="C13" s="70" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="31"/>
@@ -4092,7 +4101,9 @@
         <v>1</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="20"/>
@@ -4103,20 +4114,22 @@
       <c r="O13" s="4"/>
       <c r="P13" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="63"/>
-      <c r="C14" s="78" t="s">
-        <v>80</v>
+      <c r="B14" s="64"/>
+      <c r="C14" s="71" t="s">
+        <v>88</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="52">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="20"/>
@@ -4125,19 +4138,16 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="63"/>
-      <c r="C15" s="79" t="s">
-        <v>81</v>
+      <c r="C15" s="71" t="s">
+        <v>88</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="52">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -4156,16 +4166,18 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="63"/>
-      <c r="C16" s="78" t="s">
-        <v>82</v>
+      <c r="C16" s="72" t="s">
+        <v>89</v>
       </c>
       <c r="D16" s="31"/>
-      <c r="E16" s="53">
+      <c r="E16" s="52">
         <v>4</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <v>2</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="20"/>
       <c r="K16" s="4"/>
@@ -4175,17 +4187,17 @@
       <c r="O16" s="4"/>
       <c r="P16" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="63"/>
-      <c r="C17" s="78" t="s">
-        <v>84</v>
+      <c r="C17" s="71" t="s">
+        <v>80</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -4197,20 +4209,25 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="9"/>
+      <c r="P17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="63"/>
-      <c r="C18" s="79" t="s">
-        <v>83</v>
+      <c r="C18" s="71" t="s">
+        <v>82</v>
       </c>
       <c r="D18" s="31"/>
-      <c r="E18" s="52">
-        <v>4</v>
+      <c r="E18" s="53">
+        <v>2</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="20"/>
       <c r="K18" s="4"/>
@@ -4218,174 +4235,197 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="10">
+      <c r="P18" s="9"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="63"/>
+      <c r="C19" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="52">
+        <v>4</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>4</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="23">
-        <f>SUM(E4:E18)</f>
+      <c r="C20" s="79"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="23">
+        <f>SUM(E4:E19)</f>
         <v>34</v>
       </c>
-      <c r="F19" s="17">
-        <f t="shared" ref="F19:O19" si="1">E19-$E$19/10</f>
+      <c r="F20" s="17">
+        <f t="shared" ref="F20:O20" si="1">E20-$E$20/10</f>
         <v>30.6</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G20" s="17">
         <f t="shared" si="1"/>
         <v>27.200000000000003</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H20" s="17">
         <f t="shared" si="1"/>
         <v>23.800000000000004</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I20" s="17">
         <f t="shared" si="1"/>
         <v>20.400000000000006</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J20" s="18">
         <f t="shared" si="1"/>
         <v>17.000000000000007</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K20" s="17">
         <f t="shared" si="1"/>
         <v>13.600000000000007</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L20" s="17">
         <f t="shared" si="1"/>
         <v>10.200000000000006</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M20" s="17">
         <f t="shared" si="1"/>
         <v>6.800000000000006</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N20" s="17">
         <f t="shared" si="1"/>
         <v>3.4000000000000061</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O20" s="18">
         <f t="shared" si="1"/>
         <v>6.2172489379008766E-15</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="67" t="s">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="10">
-        <f>SUM(E4:E18)</f>
+      <c r="C21" s="79"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="10">
+        <f>SUM(E4:E19)</f>
         <v>34</v>
       </c>
-      <c r="F20" s="6">
-        <f t="shared" ref="F20:O20" si="2">E20-(SUM(F4:F18))</f>
+      <c r="F21" s="6">
+        <f t="shared" ref="F21:O21" si="2">E21-(SUM(F4:F19))</f>
         <v>27</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="H20" s="6">
+        <v>25</v>
+      </c>
+      <c r="H21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="I20" s="6">
+        <v>15</v>
+      </c>
+      <c r="I21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="J20" s="21">
+        <v>15</v>
+      </c>
+      <c r="J21" s="21">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="K20" s="6">
+        <v>15</v>
+      </c>
+      <c r="K21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="L20" s="6">
+        <v>15</v>
+      </c>
+      <c r="L21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="M20" s="6">
+        <v>15</v>
+      </c>
+      <c r="M21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="N20" s="6">
+        <v>15</v>
+      </c>
+      <c r="N21" s="6">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="O20" s="7">
+        <v>15</v>
+      </c>
+      <c r="O21" s="7">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R21" s="72"/>
+        <v>15</v>
+      </c>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R22" s="73"/>
+      <c r="R22" s="65"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R23" s="72"/>
+      <c r="R23" s="66"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R24" s="73"/>
+      <c r="R24" s="65"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R25" s="72"/>
+      <c r="R25" s="66"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R26" s="73"/>
+      <c r="R26" s="65"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R27" s="72"/>
+      <c r="R27" s="66"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R28" s="73"/>
+      <c r="R28" s="65"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R29" s="72"/>
+      <c r="R29" s="66"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R30" s="73"/>
+      <c r="R30" s="65"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R31" s="72"/>
+      <c r="R31" s="66"/>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R32" s="73"/>
+      <c r="R32" s="65"/>
     </row>
     <row r="33" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R33" s="72"/>
+      <c r="R33" s="66"/>
     </row>
     <row r="34" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R34" s="73"/>
+      <c r="R34" s="65"/>
     </row>
     <row r="35" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R35" s="72"/>
+      <c r="R35" s="66"/>
+    </row>
+    <row r="36" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R36" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4422,38 +4462,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65" t="s">
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="64" t="s">
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4509,7 +4549,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="80" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -4563,7 +4603,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="71"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -4615,7 +4655,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="80" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -4661,7 +4701,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -4705,7 +4745,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="69"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -4749,7 +4789,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="69"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -4793,7 +4833,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="69"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -4837,7 +4877,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="69"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -4881,7 +4921,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -4925,7 +4965,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -4969,7 +5009,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -5013,7 +5053,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -5057,7 +5097,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="71"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -5101,11 +5141,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -5154,11 +5194,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -5214,14 +5254,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
admin and attempting to fix button overflow on forms - mobile
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DD4FC-D2DB-48BC-BC6B-CD25B51FE696}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555EBB4E-66A5-4C90-82D3-2AF2BA9376D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -261,12 +261,6 @@
     <t>Task Viewing - shared update</t>
   </si>
   <si>
-    <t>UML Diagrams - Task creation, render, invite</t>
-  </si>
-  <si>
-    <t>UML Diagrams - Team creation, render, invite</t>
-  </si>
-  <si>
     <t>Client-side validation -User</t>
   </si>
   <si>
@@ -304,6 +298,12 @@
   </si>
   <si>
     <t>Task Creation</t>
+  </si>
+  <si>
+    <t>UML Class Diagrams - Task creation, render, invite</t>
+  </si>
+  <si>
+    <t>UML Class Diagrams - Team creation, render, invite</t>
   </si>
 </sst>
 </file>
@@ -1613,19 +1613,19 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2944,7 +2944,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="77" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
@@ -3757,7 +3757,7 @@
   <dimension ref="B1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3789,7 +3789,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="77" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
@@ -3857,7 +3857,7 @@
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="63" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="71" t="s">
         <v>70</v>
@@ -3885,7 +3885,7 @@
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="80" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="73" t="s">
         <v>71</v>
@@ -3927,10 +3927,10 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4">
+      <c r="K6" s="4">
         <v>2</v>
       </c>
+      <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -3993,12 +3993,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="82" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="60">
@@ -4013,18 +4013,20 @@
         <v>2</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>3</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="82"/>
       <c r="C10" s="68" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="53">
@@ -4039,18 +4041,20 @@
         <v>2</v>
       </c>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>3</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="62">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="82"/>
       <c r="C11" s="69" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="52">
@@ -4076,7 +4080,7 @@
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="82"/>
       <c r="C12" s="68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="52">
@@ -4104,7 +4108,7 @@
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="82"/>
       <c r="C13" s="70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="52">
@@ -4132,7 +4136,7 @@
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="64"/>
       <c r="C14" s="71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="52">
@@ -4155,7 +4159,7 @@
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="63"/>
       <c r="C15" s="71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="52">
@@ -4179,7 +4183,7 @@
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="63"/>
       <c r="C16" s="72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="52">
@@ -4192,10 +4196,10 @@
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4">
+      <c r="K16" s="4">
         <v>6</v>
       </c>
+      <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -4207,7 +4211,7 @@
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="63"/>
       <c r="C17" s="71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="53">
@@ -4231,7 +4235,7 @@
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="63"/>
       <c r="C18" s="71" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" s="31"/>
       <c r="E18" s="53">
@@ -4254,7 +4258,7 @@
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="63"/>
       <c r="C19" s="72" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19" s="31"/>
       <c r="E19" s="52">
@@ -4339,44 +4343,44 @@
         <v>34</v>
       </c>
       <c r="F21" s="6">
-        <f>E21-(SUM(F4:F19))</f>
+        <f t="shared" ref="F21:O21" si="2">E21-(SUM(F4:F19))</f>
         <v>27</v>
       </c>
       <c r="G21" s="6">
-        <f>F21-(SUM(G4:G19))</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="H21" s="6">
-        <f>G21-(SUM(H4:H19))</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I21" s="6">
-        <f>H21-(SUM(I4:I19))</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J21" s="21">
-        <f>I21-(SUM(J4:J19))</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="K21" s="6">
-        <f>J21-(SUM(K4:K19))</f>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>-1</v>
       </c>
       <c r="L21" s="6">
-        <f>K21-(SUM(L4:L19))</f>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
       <c r="M21" s="6">
-        <f>L21-(SUM(M4:M19))</f>
-        <v>-1</v>
+        <f t="shared" si="2"/>
+        <v>-7</v>
       </c>
       <c r="N21" s="6">
-        <f>M21-(SUM(N4:N19))</f>
-        <v>-1</v>
+        <f t="shared" si="2"/>
+        <v>-7</v>
       </c>
       <c r="O21" s="7">
-        <f>N21-(SUM(O4:O19))</f>
-        <v>-1</v>
+        <f t="shared" si="2"/>
+        <v>-7</v>
       </c>
       <c r="P21" s="8"/>
       <c r="Q21" s="2"/>
@@ -4432,14 +4436,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5268,14 +5272,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added completion mechanics to the task tile added the ability for teams to defined their own experience types.
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555EBB4E-66A5-4C90-82D3-2AF2BA9376D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EDE1AD-3FB8-4182-B95B-DF1282D2CCC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29130" yWindow="690" windowWidth="28200" windowHeight="14085" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
     <sheet name="Sprint Backlog 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sprint Backlog 1 (2)" sheetId="6" r:id="rId3"/>
-    <sheet name="Sprint Backlog 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint Backlog2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sprint Backlog 3" sheetId="7" r:id="rId4"/>
+    <sheet name="Sprint Backlog example" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
   <si>
     <t>Task</t>
   </si>
@@ -304,15 +305,88 @@
   </si>
   <si>
     <t>UML Class Diagrams - Team creation, render, invite</t>
+  </si>
+  <si>
+    <t>VIVA</t>
+  </si>
+  <si>
+    <t>UML Sequence Diagrams - team creation, render, invite</t>
+  </si>
+  <si>
+    <t>UML Sequence Diagrams - task creation, render</t>
+  </si>
+  <si>
+    <t>Client-side validation -Teams</t>
+  </si>
+  <si>
+    <t>Database Schema</t>
+  </si>
+  <si>
+    <t>Task Completion(TC) - change status</t>
+  </si>
+  <si>
+    <r>
+      <t>TC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - respect requirements</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - UI control</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - give experience rewards</t>
+    </r>
+  </si>
+  <si>
+    <t>Supervisor Meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -710,139 +784,139 @@
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -851,130 +925,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -985,20 +1062,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1450,7 +1530,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint Backlog 1 (2)'!$E$3:$O$3</c:f>
+              <c:f>'Sprint Backlog2'!$E$3:$O$3</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1491,42 +1571,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1 (2)'!$E$20:$O$20</c:f>
+              <c:f>'Sprint Backlog2'!$E$21:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>34</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.6</c:v>
+                  <c:v>31.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.200000000000003</c:v>
+                  <c:v>27.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.800000000000004</c:v>
+                  <c:v>24.150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.400000000000006</c:v>
+                  <c:v>20.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.000000000000007</c:v>
+                  <c:v>17.250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.600000000000007</c:v>
+                  <c:v>13.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.200000000000006</c:v>
+                  <c:v>10.350000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.800000000000006</c:v>
+                  <c:v>6.9000000000000048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4000000000000061</c:v>
+                  <c:v>3.4500000000000046</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.2172489379008766E-15</c:v>
+                  <c:v>4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1549,7 +1629,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint Backlog 1 (2)'!$E$3:$O$3</c:f>
+              <c:f>'Sprint Backlog2'!$E$3:$O$3</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1590,42 +1670,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1 (2)'!$E$21:$O$21</c:f>
+              <c:f>'Sprint Backlog2'!$E$22:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-7</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-7</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1764,6 +1844,340 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
+          <c:x val="0.16282253282832151"/>
+          <c:y val="1.8470584658792262E-2"/>
+          <c:w val="0.71469100453352397"/>
+          <c:h val="0.79831147760594201"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 3'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 3'!$E$16:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0929-4D7A-A4FA-3FE4F933C78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 3'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 3'!$E$17:$O$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0929-4D7A-A4FA-3FE4F933C78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="132299304"/>
+        <c:axId val="132299696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="132299304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DAYS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="132299696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>HOURS EFFORT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
           <c:x val="0.13306959254568099"/>
           <c:y val="1.8470685733562999E-2"/>
           <c:w val="0.71469100453352397"/>
@@ -1784,7 +2198,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint Backlog 2'!$G$3:$Q$3</c:f>
+              <c:f>'Sprint Backlog example'!$G$3:$Q$3</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1883,7 +2297,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint Backlog 2'!$G$3:$Q$3</c:f>
+              <c:f>'Sprint Backlog example'!$G$3:$Q$3</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1924,7 +2338,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 2'!$G$18:$Q$18</c:f>
+              <c:f>'Sprint Backlog example'!$G$18:$Q$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2124,13 +2538,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>475111</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>131724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>252860</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2162,6 +2576,49 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>475111</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>131724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>252860</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121138</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C913A5E4-4D2C-4A24-9B2A-124287022D87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2529,7 +2986,7 @@
   <dimension ref="B1:G31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2934,34 +3391,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="76" t="s">
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3011,7 +3468,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="83" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="54" t="s">
@@ -3057,7 +3514,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="82"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="57" t="s">
         <v>65</v>
       </c>
@@ -3101,7 +3558,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="82"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="56" t="s">
         <v>61</v>
       </c>
@@ -3145,7 +3602,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="82"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -3185,7 +3642,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="81" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="61" t="s">
@@ -3231,7 +3688,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="81"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="57" t="s">
         <v>67</v>
       </c>
@@ -3275,7 +3732,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="81"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="59" t="s">
         <v>60</v>
       </c>
@@ -3319,7 +3776,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="81"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="56" t="s">
         <v>57</v>
       </c>
@@ -3363,7 +3820,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="81"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="54" t="s">
         <v>58</v>
       </c>
@@ -3407,7 +3864,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="54" t="s">
         <v>69</v>
       </c>
@@ -3451,7 +3908,7 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="54" t="s">
         <v>68</v>
       </c>
@@ -3493,7 +3950,7 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="83"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="56" t="s">
         <v>59</v>
       </c>
@@ -3537,7 +3994,7 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="81" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="54" t="s">
@@ -3583,7 +4040,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="81"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="54" t="s">
         <v>63</v>
       </c>
@@ -3627,10 +4084,10 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="32"/>
       <c r="E18" s="23">
         <f>SUM(E4:E17)</f>
@@ -3678,10 +4135,10 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="79"/>
+      <c r="C19" s="80"/>
       <c r="D19" s="33"/>
       <c r="E19" s="10">
         <f>SUM(E4:E17)</f>
@@ -3754,10 +4211,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E71DFC-EBA7-4F4A-8776-6F171A9158CA}">
-  <dimension ref="B1:U36"/>
+  <dimension ref="B1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3779,34 +4236,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="76" t="s">
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3884,7 +4341,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="81" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="73" t="s">
@@ -3907,12 +4364,12 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P19" si="0">SUM(F5:O5)</f>
+        <f t="shared" ref="P5:P20" si="0">SUM(F5:O5)</f>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
+      <c r="B6" s="82"/>
       <c r="C6" s="65" t="s">
         <v>72</v>
       </c>
@@ -3940,7 +4397,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="81"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="66" t="s">
         <v>73</v>
       </c>
@@ -3968,7 +4425,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="83"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="65" t="s">
         <v>74</v>
       </c>
@@ -3994,7 +4451,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="83" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="67" t="s">
@@ -4009,9 +4466,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="20"/>
-      <c r="K9" s="4">
-        <v>2</v>
-      </c>
+      <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4">
         <v>3</v>
@@ -4020,11 +4475,11 @@
       <c r="O9" s="4"/>
       <c r="P9" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="82"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="68" t="s">
         <v>89</v>
       </c>
@@ -4037,9 +4492,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="20"/>
-      <c r="K10" s="4">
-        <v>2</v>
-      </c>
+      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4">
         <v>3</v>
@@ -4048,11 +4501,11 @@
       <c r="O10" s="4"/>
       <c r="P10" s="62">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="82"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="69" t="s">
         <v>75</v>
       </c>
@@ -4065,20 +4518,18 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="20"/>
-      <c r="K11" s="4">
-        <v>2</v>
-      </c>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="82"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="68" t="s">
         <v>76</v>
       </c>
@@ -4093,20 +4544,18 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="20"/>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
+      <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="70" t="s">
         <v>77</v>
       </c>
@@ -4116,36 +4565,721 @@
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="20"/>
-      <c r="K13" s="4">
-        <v>1</v>
-      </c>
+      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="9">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="64"/>
-      <c r="C14" s="71" t="s">
-        <v>86</v>
+      <c r="B14" s="76"/>
+      <c r="C14" s="85" t="s">
+        <v>90</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="52">
         <v>0.5</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4">
         <v>0.5</v>
       </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="9">
+        <f t="shared" ref="P14" si="1">SUM(F14:O14)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="64"/>
+      <c r="C15" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="63"/>
+      <c r="C16" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="63"/>
+      <c r="C17" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="52">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="4">
+        <v>6</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="63"/>
+      <c r="C18" s="71" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="53">
+        <v>4</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="63"/>
+      <c r="C19" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="53">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="9"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="63"/>
+      <c r="C20" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="52">
+        <v>4</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4">
+        <v>4</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="80"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="23">
+        <f>SUM(E4:E20)</f>
+        <v>34.5</v>
+      </c>
+      <c r="F21" s="17">
+        <f t="shared" ref="F21:O21" si="2">E21-$E$21/10</f>
+        <v>31.05</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="2"/>
+        <v>27.6</v>
+      </c>
+      <c r="H21" s="17">
+        <f t="shared" si="2"/>
+        <v>24.150000000000002</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" si="2"/>
+        <v>20.700000000000003</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="2"/>
+        <v>17.250000000000004</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="2"/>
+        <v>13.800000000000004</v>
+      </c>
+      <c r="L21" s="17">
+        <f t="shared" si="2"/>
+        <v>10.350000000000005</v>
+      </c>
+      <c r="M21" s="17">
+        <f t="shared" si="2"/>
+        <v>6.9000000000000048</v>
+      </c>
+      <c r="N21" s="17">
+        <f t="shared" si="2"/>
+        <v>3.4500000000000046</v>
+      </c>
+      <c r="O21" s="18">
+        <f t="shared" si="2"/>
+        <v>4.4408920985006262E-15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="10">
+        <f>SUM(E4:E20)</f>
+        <v>34.5</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22:O22" si="3">E22-(SUM(F4:F20))</f>
+        <v>27.5</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="H22" s="6">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="3"/>
+        <v>13.5</v>
+      </c>
+      <c r="J22" s="21">
+        <f t="shared" si="3"/>
+        <v>13.5</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="3"/>
+        <v>5.5</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="3"/>
+        <v>5.5</v>
+      </c>
+      <c r="M22" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.5</v>
+      </c>
+      <c r="N22" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.5</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="3"/>
+        <v>-0.5</v>
+      </c>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R23" s="65"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R24" s="66"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R25" s="65"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R26" s="66"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R27" s="65"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R28" s="66"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R29" s="65"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R30" s="66"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R31" s="65"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R32" s="66"/>
+    </row>
+    <row r="33" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R33" s="65"/>
+    </row>
+    <row r="34" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R34" s="66"/>
+    </row>
+    <row r="35" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R35" s="65"/>
+    </row>
+    <row r="36" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R36" s="66"/>
+    </row>
+    <row r="37" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R37" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="B21:C21"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF3C117-F50E-4201-8F00-39D353D27E11}">
+  <dimension ref="B1:U32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="7" width="7.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="7" style="5" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7.625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="5.875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+    </row>
+    <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="51">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="23">
+        <f>SUM(F4:O4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="9">
+        <f t="shared" ref="P5:P12" si="0">SUM(F5:O5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="82"/>
+      <c r="C6" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="53">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="82"/>
+      <c r="C7" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="52">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="82"/>
+      <c r="C8" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="60">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="84"/>
+      <c r="C9" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="60">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="83" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="60">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="83"/>
+      <c r="C11" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="53">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="83"/>
+      <c r="C12" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="52">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="76"/>
+      <c r="C13" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="76"/>
+      <c r="C14" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="20"/>
@@ -4157,13 +5291,13 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="63"/>
-      <c r="C15" s="71" t="s">
-        <v>86</v>
+      <c r="B15" s="76"/>
+      <c r="C15" s="65" t="s">
+        <v>78</v>
       </c>
       <c r="D15" s="31"/>
-      <c r="E15" s="52">
-        <v>0.5</v>
+      <c r="E15" s="60">
+        <v>6</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -4175,219 +5309,127 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="63"/>
-      <c r="C16" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="52">
+      <c r="B16" s="80" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="80"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="23">
+        <f>SUM(E4:E15)</f>
+        <v>32.5</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" ref="F16:O16" si="1">E16-$E$16/10</f>
+        <v>29.25</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H16" s="17">
+        <f t="shared" si="1"/>
+        <v>22.75</v>
+      </c>
+      <c r="I16" s="17">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="J16" s="18">
+        <f t="shared" si="1"/>
+        <v>16.25</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L16" s="17">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="N16" s="17">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
+      </c>
+      <c r="O16" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4">
-        <v>2</v>
-      </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="4">
-        <v>6</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="63"/>
-      <c r="C17" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="53">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="C17" s="80"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="10">
+        <f>SUM(E4:E15)</f>
+        <v>32.5</v>
+      </c>
+      <c r="F17" s="6">
+        <f>E17-(SUM(F4:F12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="G17" s="6">
+        <f>F17-(SUM(G4:G12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="H17" s="6">
+        <f>G17-(SUM(H4:H12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="I17" s="6">
+        <f>H17-(SUM(I4:I12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="J17" s="21">
+        <f>I17-(SUM(J4:J12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="K17" s="6">
+        <f>J17-(SUM(K4:K12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="L17" s="6">
+        <f>K17-(SUM(L4:L12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="M17" s="6">
+        <f>L17-(SUM(M4:M12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="N17" s="6">
+        <f>M17-(SUM(N4:N12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="O17" s="7">
+        <f>N17-(SUM(O4:O12))</f>
+        <v>30.5</v>
+      </c>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="63"/>
-      <c r="C18" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="53">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4">
-        <v>1</v>
-      </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="9"/>
+      <c r="R18" s="65"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="63"/>
-      <c r="C19" s="72" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="52">
-        <v>4</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4">
-        <v>4</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="10">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+      <c r="R19" s="66"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="23">
-        <f>SUM(E4:E19)</f>
-        <v>34</v>
-      </c>
-      <c r="F20" s="17">
-        <f t="shared" ref="F20:O20" si="1">E20-$E$20/10</f>
-        <v>30.6</v>
-      </c>
-      <c r="G20" s="17">
-        <f t="shared" si="1"/>
-        <v>27.200000000000003</v>
-      </c>
-      <c r="H20" s="17">
-        <f t="shared" si="1"/>
-        <v>23.800000000000004</v>
-      </c>
-      <c r="I20" s="17">
-        <f t="shared" si="1"/>
-        <v>20.400000000000006</v>
-      </c>
-      <c r="J20" s="18">
-        <f t="shared" si="1"/>
-        <v>17.000000000000007</v>
-      </c>
-      <c r="K20" s="17">
-        <f t="shared" si="1"/>
-        <v>13.600000000000007</v>
-      </c>
-      <c r="L20" s="17">
-        <f t="shared" si="1"/>
-        <v>10.200000000000006</v>
-      </c>
-      <c r="M20" s="17">
-        <f t="shared" si="1"/>
-        <v>6.800000000000006</v>
-      </c>
-      <c r="N20" s="17">
-        <f t="shared" si="1"/>
-        <v>3.4000000000000061</v>
-      </c>
-      <c r="O20" s="18">
-        <f t="shared" si="1"/>
-        <v>6.2172489379008766E-15</v>
-      </c>
+      <c r="R20" s="65"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="10">
-        <f>SUM(E4:E19)</f>
-        <v>34</v>
-      </c>
-      <c r="F21" s="6">
-        <f t="shared" ref="F21:O21" si="2">E21-(SUM(F4:F19))</f>
-        <v>27</v>
-      </c>
-      <c r="G21" s="6">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="H21" s="6">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="I21" s="6">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="J21" s="21">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="K21" s="6">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="L21" s="6">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="M21" s="6">
-        <f t="shared" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="N21" s="6">
-        <f t="shared" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="O21" s="7">
-        <f t="shared" si="2"/>
-        <v>-7</v>
-      </c>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
+      <c r="R21" s="66"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R22" s="65"/>
@@ -4422,28 +5464,16 @@
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R32" s="65"/>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R33" s="66"/>
-    </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R34" s="65"/>
-    </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R35" s="66"/>
-    </row>
-    <row r="36" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R36" s="65"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4451,12 +5481,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:W18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="B2:R18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4480,38 +5510,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="76" t="s">
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4567,7 +5597,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="81" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -4621,7 +5651,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -4673,7 +5703,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="81" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -4719,7 +5749,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="81"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -4763,7 +5793,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="81"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -4807,7 +5837,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="81"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -4851,7 +5881,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="81"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -4895,7 +5925,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="81"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -4939,7 +5969,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="81"/>
+      <c r="B12" s="82"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -4983,7 +6013,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -5027,7 +6057,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -5071,7 +6101,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="81"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -5115,7 +6145,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="83"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -5159,11 +6189,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -5212,11 +6242,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -5272,14 +6302,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
just documenting process in the new task by task format, adding task durations to the plan
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EDE1AD-3FB8-4182-B95B-DF1282D2CCC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97BFF1B-39AA-4B69-B654-26E9A0E74F35}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29130" yWindow="690" windowWidth="28200" windowHeight="14085" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28200" windowHeight="14085" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -1053,6 +1053,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1076,9 +1079,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -2015,31 +2015,31 @@
                   <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30.5</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3391,34 +3391,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="77" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3468,7 +3468,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="54" t="s">
@@ -3514,7 +3514,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="83"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="57" t="s">
         <v>65</v>
       </c>
@@ -3558,7 +3558,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="83"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="56" t="s">
         <v>61</v>
       </c>
@@ -3602,7 +3602,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="83"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -3642,7 +3642,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="82" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="61" t="s">
@@ -3688,7 +3688,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="82"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="57" t="s">
         <v>67</v>
       </c>
@@ -3732,7 +3732,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="82"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="59" t="s">
         <v>60</v>
       </c>
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="82"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="56" t="s">
         <v>57</v>
       </c>
@@ -3820,7 +3820,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="82"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="54" t="s">
         <v>58</v>
       </c>
@@ -3864,7 +3864,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="54" t="s">
         <v>69</v>
       </c>
@@ -3908,7 +3908,7 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="82"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="54" t="s">
         <v>68</v>
       </c>
@@ -3950,7 +3950,7 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="84"/>
+      <c r="B15" s="85"/>
       <c r="C15" s="56" t="s">
         <v>59</v>
       </c>
@@ -3994,7 +3994,7 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="54" t="s">
@@ -4040,7 +4040,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="82"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="54" t="s">
         <v>63</v>
       </c>
@@ -4084,10 +4084,10 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="80"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="32"/>
       <c r="E18" s="23">
         <f>SUM(E4:E17)</f>
@@ -4135,10 +4135,10 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="80"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="33"/>
       <c r="E19" s="10">
         <f>SUM(E4:E17)</f>
@@ -4236,34 +4236,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="77" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4341,7 +4341,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="82" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="73" t="s">
@@ -4369,7 +4369,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="82"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="65" t="s">
         <v>72</v>
       </c>
@@ -4397,7 +4397,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="82"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="66" t="s">
         <v>73</v>
       </c>
@@ -4425,7 +4425,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="84"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="65" t="s">
         <v>74</v>
       </c>
@@ -4451,7 +4451,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="84" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="67" t="s">
@@ -4479,7 +4479,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="83"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="68" t="s">
         <v>89</v>
       </c>
@@ -4505,7 +4505,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="69" t="s">
         <v>75</v>
       </c>
@@ -4529,7 +4529,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="68" t="s">
         <v>76</v>
       </c>
@@ -4555,7 +4555,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="83"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="70" t="s">
         <v>77</v>
       </c>
@@ -4582,7 +4582,7 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="76"/>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="77" t="s">
         <v>90</v>
       </c>
       <c r="D14" s="31"/>
@@ -4755,10 +4755,10 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="80"/>
+      <c r="C21" s="81"/>
       <c r="D21" s="32"/>
       <c r="E21" s="23">
         <f>SUM(E4:E20)</f>
@@ -4806,10 +4806,10 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="80"/>
+      <c r="C22" s="81"/>
       <c r="D22" s="33"/>
       <c r="E22" s="10">
         <f>SUM(E4:E20)</f>
@@ -4909,14 +4909,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4929,7 +4929,7 @@
   <dimension ref="B1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4951,34 +4951,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="77" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5056,7 +5056,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="82" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="66" t="s">
@@ -5067,7 +5067,9 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="20"/>
@@ -5078,11 +5080,11 @@
       <c r="O5" s="4"/>
       <c r="P5" s="9">
         <f t="shared" ref="P5:P12" si="0">SUM(F5:O5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="82"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="66" t="s">
         <v>95</v>
       </c>
@@ -5091,7 +5093,9 @@
         <v>2</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="20"/>
@@ -5102,11 +5106,11 @@
       <c r="O6" s="4"/>
       <c r="P6" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="82"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="65" t="s">
         <v>96</v>
       </c>
@@ -5130,7 +5134,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="82"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="65" t="s">
         <v>98</v>
       </c>
@@ -5139,7 +5143,9 @@
         <v>6</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="20"/>
@@ -5151,7 +5157,7 @@
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="84"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="66" t="s">
         <v>97</v>
       </c>
@@ -5160,7 +5166,9 @@
         <v>1</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="20"/>
@@ -5171,11 +5179,11 @@
       <c r="O9" s="4"/>
       <c r="P9" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="84" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="66" t="s">
@@ -5201,7 +5209,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="83"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="65" t="s">
         <v>92</v>
       </c>
@@ -5225,7 +5233,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="83"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="65" t="s">
         <v>94</v>
       </c>
@@ -5312,10 +5320,10 @@
       <c r="P15" s="10"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="80"/>
+      <c r="C16" s="81"/>
       <c r="D16" s="32"/>
       <c r="E16" s="23">
         <f>SUM(E4:E15)</f>
@@ -5363,54 +5371,54 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="80"/>
+      <c r="C17" s="81"/>
       <c r="D17" s="33"/>
       <c r="E17" s="10">
         <f>SUM(E4:E15)</f>
         <v>32.5</v>
       </c>
       <c r="F17" s="6">
-        <f>E17-(SUM(F4:F12))</f>
+        <f t="shared" ref="F17:O17" si="2">E17-(SUM(F4:F12))</f>
         <v>30.5</v>
       </c>
       <c r="G17" s="6">
-        <f>F17-(SUM(G4:G12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="H17" s="6">
-        <f>G17-(SUM(H4:H12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="I17" s="6">
-        <f>H17-(SUM(I4:I12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="J17" s="21">
-        <f>I17-(SUM(J4:J12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="K17" s="6">
-        <f>J17-(SUM(K4:K12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="L17" s="6">
-        <f>K17-(SUM(L4:L12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="M17" s="6">
-        <f>L17-(SUM(M4:M12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="N17" s="6">
-        <f>M17-(SUM(N4:N12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="O17" s="7">
-        <f>N17-(SUM(O4:O12))</f>
-        <v>30.5</v>
+        <f t="shared" si="2"/>
+        <v>21.5</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="2"/>
@@ -5466,14 +5474,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5510,38 +5518,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78" t="s">
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="77" t="s">
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5597,7 +5605,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -5651,7 +5659,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="84"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -5703,7 +5711,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="82" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -5749,7 +5757,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="82"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -5793,7 +5801,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="82"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -5837,7 +5845,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="82"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -5881,7 +5889,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="82"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -5925,7 +5933,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="82"/>
+      <c r="B11" s="83"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -5969,7 +5977,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="82"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -6013,7 +6021,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="82"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -6057,7 +6065,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="82"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -6101,7 +6109,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="82"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -6145,7 +6153,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="84"/>
+      <c r="B16" s="85"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -6189,11 +6197,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -6242,11 +6250,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -6302,14 +6310,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fixed bug with empty additional skills collecton fixed UX style with card spacing fixed jquery button styling inconsistancy added a few extra divs for card wrapping added fanfare mechanic to trigger notify on the screen center (concider moving to navbar elements)
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88292454-2139-46AB-B8D3-A68E2B58A128}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFA9100-8AD5-40AF-B81C-BCC31CACBEB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1545" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Sprint Backlog2" sheetId="6" r:id="rId3"/>
     <sheet name="Sprint Backlog 3" sheetId="7" r:id="rId4"/>
     <sheet name="Sprint Backlog 4" sheetId="8" r:id="rId5"/>
-    <sheet name="Sprint Backlog example" sheetId="4" r:id="rId6"/>
+    <sheet name="Sprint Backlog 5" sheetId="9" r:id="rId6"/>
+    <sheet name="Sprint Backlog example" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
   <si>
     <t>Task</t>
   </si>
@@ -374,9 +375,6 @@
     <t>Supervisor Meeting</t>
   </si>
   <si>
-    <t>UX Form Tooltips</t>
-  </si>
-  <si>
     <t>UX Task Completion Failure</t>
   </si>
   <si>
@@ -393,6 +391,42 @@
   </si>
   <si>
     <t>Finialise Aditional Features List</t>
+  </si>
+  <si>
+    <t>16/12/2019-03/01/2020</t>
+  </si>
+  <si>
+    <t>UX form helptext</t>
+  </si>
+  <si>
+    <t>UX Form Input labels</t>
+  </si>
+  <si>
+    <t>New User skill-list empty</t>
+  </si>
+  <si>
+    <t>Sprint planning</t>
+  </si>
+  <si>
+    <t>Supervisor meeting x2</t>
+  </si>
+  <si>
+    <t>User Page Experience Update</t>
+  </si>
+  <si>
+    <t>Conduct Survey</t>
+  </si>
+  <si>
+    <t>Fanfare mechanic</t>
+  </si>
+  <si>
+    <t>Level-up fanfair</t>
+  </si>
+  <si>
+    <t>Skill Icons</t>
+  </si>
+  <si>
+    <t>Information Arechecture</t>
   </si>
 </sst>
 </file>
@@ -871,7 +905,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1096,32 +1130,56 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1280,39 +1338,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$18:$O$18</c:f>
+              <c:f>'Sprint Backlog 1'!$E$19:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>47.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.75</c:v>
+                  <c:v>45.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>40.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.25</c:v>
+                  <c:v>35.350000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.5</c:v>
+                  <c:v>30.300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.75</c:v>
+                  <c:v>25.250000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>20.200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.25</c:v>
+                  <c:v>15.150000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5</c:v>
+                  <c:v>10.100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.75</c:v>
+                  <c:v>5.0500000000000052</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1379,33 +1437,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$19:$O$19</c:f>
+              <c:f>'Sprint Backlog 1'!$E$20:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>47.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.5</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-1</c:v>
@@ -1614,42 +1672,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog2'!$E$21:$O$21</c:f>
+              <c:f>'Sprint Backlog2'!$E$22:$O$22</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>34.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.05</c:v>
+                  <c:v>33.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.6</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.150000000000002</c:v>
+                  <c:v>26.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.700000000000003</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.250000000000004</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.800000000000004</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.350000000000005</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9000000000000048</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4500000000000046</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4408920985006262E-15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1713,42 +1771,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog2'!$E$22:$O$22</c:f>
+              <c:f>'Sprint Backlog2'!$E$23:$O$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1948,42 +2006,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 3'!$E$16:$O$16</c:f>
+              <c:f>'Sprint Backlog 3'!$E$17:$O$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>30.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.45</c:v>
+                  <c:v>28.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.4</c:v>
+                  <c:v>25.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.349999999999998</c:v>
+                  <c:v>22.050000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.299999999999997</c:v>
+                  <c:v>18.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.249999999999996</c:v>
+                  <c:v>15.750000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.199999999999996</c:v>
+                  <c:v>12.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.149999999999995</c:v>
+                  <c:v>9.4500000000000046</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0999999999999952</c:v>
+                  <c:v>6.3000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0499999999999954</c:v>
+                  <c:v>3.1500000000000044</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-4.4408920985006262E-15</c:v>
+                  <c:v>4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2047,42 +2105,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 3'!$E$17:$O$17</c:f>
+              <c:f>'Sprint Backlog 3'!$E$18:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>30.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.5</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.5</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2282,42 +2340,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 4'!$E$12:$O$12</c:f>
+              <c:f>'Sprint Backlog 4'!$E$14:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>27.5</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.75</c:v>
+                  <c:v>22.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.25</c:v>
+                  <c:v>17.150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.5</c:v>
+                  <c:v>14.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.75</c:v>
+                  <c:v>12.250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>9.8000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.25</c:v>
+                  <c:v>7.3500000000000041</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.5</c:v>
+                  <c:v>4.9000000000000039</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.75</c:v>
+                  <c:v>2.4500000000000037</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3.5527136788005009E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2381,42 +2439,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 4'!$E$13:$O$13</c:f>
+              <c:f>'Sprint Backlog 4'!$E$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>27.5</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2555,6 +2613,340 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
+          <c:x val="0.16282253282832151"/>
+          <c:y val="1.8470584658792262E-2"/>
+          <c:w val="0.71469100453352397"/>
+          <c:h val="0.79831147760594201"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 5'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 5'!$E$13:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.650000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.9000000000000048</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9500000000000046</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4408920985006262E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-27D3-478F-9835-913D6D3AB8C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 5'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 5'!$E$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-27D3-478F-9835-913D6D3AB8C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="132299304"/>
+        <c:axId val="132299696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="132299304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DAYS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="132299696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>HOURS EFFORT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
           <c:x val="0.13306959254568099"/>
           <c:y val="1.8470685733562999E-2"/>
           <c:w val="0.71469100453352397"/>
@@ -2616,39 +3008,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 1'!$E$18:$O$18</c:f>
+              <c:f>'Sprint Backlog 1'!$E$19:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>47.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.75</c:v>
+                  <c:v>45.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>40.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.25</c:v>
+                  <c:v>35.350000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.5</c:v>
+                  <c:v>30.300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.75</c:v>
+                  <c:v>25.250000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>20.200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.25</c:v>
+                  <c:v>15.150000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5</c:v>
+                  <c:v>10.100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.75</c:v>
+                  <c:v>5.0500000000000052</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2874,13 +3266,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>467784</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>80435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>245533</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2915,13 +3307,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>475111</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>131724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>252860</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2958,13 +3350,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>475111</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>131724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>252860</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3001,13 +3393,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>475111</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>131724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>252860</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3039,6 +3431,49 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>475111</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>131724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>252860</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>121138</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{309E0270-D6DD-402E-B93C-0C1AB6CB59BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3786,10 +4221,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:U19"/>
+  <dimension ref="B1:U20"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3811,34 +4246,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="83" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -3888,7 +4323,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="95" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="54" t="s">
@@ -3934,7 +4369,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="89"/>
+      <c r="B5" s="95"/>
       <c r="C5" s="57" t="s">
         <v>65</v>
       </c>
@@ -3973,12 +4408,12 @@
         <v>0</v>
       </c>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P17" si="0">SUM(F5:O5)</f>
+        <f t="shared" ref="P5:P18" si="0">SUM(F5:O5)</f>
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="89"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="56" t="s">
         <v>61</v>
       </c>
@@ -4022,7 +4457,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="89"/>
+      <c r="B7" s="95"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -4062,7 +4497,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="93" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="61" t="s">
@@ -4108,7 +4543,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="88"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="57" t="s">
         <v>67</v>
       </c>
@@ -4152,7 +4587,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="88"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="59" t="s">
         <v>60</v>
       </c>
@@ -4196,7 +4631,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="88"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="56" t="s">
         <v>57</v>
       </c>
@@ -4240,7 +4675,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="88"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="54" t="s">
         <v>58</v>
       </c>
@@ -4284,7 +4719,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="88"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="54" t="s">
         <v>69</v>
       </c>
@@ -4328,7 +4763,7 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="88"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="54" t="s">
         <v>68</v>
       </c>
@@ -4370,7 +4805,7 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="90"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="56" t="s">
         <v>59</v>
       </c>
@@ -4414,39 +4849,33 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="87" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>62</v>
+      <c r="B16" s="82"/>
+      <c r="C16" s="56" t="s">
+        <v>103</v>
       </c>
       <c r="D16" s="31"/>
-      <c r="E16" s="53">
+      <c r="E16" s="60">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4">
         <v>0.5</v>
       </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
         <v>0.5</v>
       </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="20">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K16" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L16" s="4">
         <v>0.5</v>
       </c>
       <c r="M16" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N16" s="4">
         <v>0</v>
@@ -4454,172 +4883,218 @@
       <c r="O16" s="4">
         <v>0</v>
       </c>
-      <c r="P16" s="9">
+      <c r="P16" s="62">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="20">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="88"/>
-      <c r="C17" s="54" t="s">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="94"/>
+      <c r="C18" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="52">
+      <c r="D18" s="31"/>
+      <c r="E18" s="52">
         <v>0.5</v>
       </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="20">
-        <v>0</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <v>0</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17" s="4">
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="86" t="s">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="23">
-        <f>SUM(E4:E17)</f>
-        <v>47.5</v>
-      </c>
-      <c r="F18" s="17">
-        <f t="shared" ref="F18:O18" si="2">E18-$E$18/10</f>
-        <v>42.75</v>
-      </c>
-      <c r="G18" s="17">
+      <c r="C19" s="92"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="23">
+        <f>SUM(E4:E18)</f>
+        <v>50.5</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" ref="F19:O19" si="2">E19-$E$19/10</f>
+        <v>45.45</v>
+      </c>
+      <c r="G19" s="17">
         <f t="shared" si="2"/>
+        <v>40.400000000000006</v>
+      </c>
+      <c r="H19" s="17">
+        <f t="shared" si="2"/>
+        <v>35.350000000000009</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="2"/>
+        <v>30.300000000000008</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="2"/>
+        <v>25.250000000000007</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="2"/>
+        <v>20.200000000000006</v>
+      </c>
+      <c r="L19" s="17">
+        <f t="shared" si="2"/>
+        <v>15.150000000000006</v>
+      </c>
+      <c r="M19" s="17">
+        <f t="shared" si="2"/>
+        <v>10.100000000000005</v>
+      </c>
+      <c r="N19" s="17">
+        <f t="shared" si="2"/>
+        <v>5.0500000000000052</v>
+      </c>
+      <c r="O19" s="18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="92"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="10">
+        <f>SUM(E4:E18)</f>
+        <v>50.5</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" ref="F20:O20" si="3">E20-(SUM(F4:F18))</f>
+        <v>38.5</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="H18" s="17">
-        <f t="shared" si="2"/>
-        <v>33.25</v>
-      </c>
-      <c r="I18" s="17">
-        <f t="shared" si="2"/>
-        <v>28.5</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="2"/>
-        <v>23.75</v>
-      </c>
-      <c r="K18" s="17">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="L18" s="17">
-        <f t="shared" si="2"/>
-        <v>14.25</v>
-      </c>
-      <c r="M18" s="17">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
-      </c>
-      <c r="N18" s="17">
-        <f t="shared" si="2"/>
-        <v>4.75</v>
-      </c>
-      <c r="O18" s="18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="10">
-        <f>SUM(E4:E17)</f>
-        <v>47.5</v>
-      </c>
-      <c r="F19" s="6">
-        <f t="shared" ref="F19:O19" si="3">E19-(SUM(F4:F17))</f>
-        <v>36</v>
-      </c>
-      <c r="G19" s="6">
+      <c r="H20" s="6">
         <f t="shared" si="3"/>
-        <v>35.5</v>
-      </c>
-      <c r="H19" s="6">
+        <v>23.5</v>
+      </c>
+      <c r="I20" s="6">
         <f t="shared" si="3"/>
-        <v>21.5</v>
-      </c>
-      <c r="I19" s="6">
+        <v>23.5</v>
+      </c>
+      <c r="J20" s="21">
         <f t="shared" si="3"/>
-        <v>21.5</v>
-      </c>
-      <c r="J19" s="21">
+        <v>20</v>
+      </c>
+      <c r="K20" s="6">
         <f t="shared" si="3"/>
-        <v>18.5</v>
-      </c>
-      <c r="K19" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="L20" s="6">
         <f t="shared" si="3"/>
-        <v>11.5</v>
-      </c>
-      <c r="L19" s="6">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="M19" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="M20" s="6">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="N19" s="6">
+      <c r="N20" s="6">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O20" s="7">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C1:F1"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
     <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B8:B15"/>
   </mergeCells>
@@ -4631,10 +5106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E71DFC-EBA7-4F4A-8776-6F171A9158CA}">
-  <dimension ref="B1:U37"/>
+  <dimension ref="B1:U38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4656,34 +5131,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="83" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4761,7 +5236,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="93" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="73" t="s">
@@ -4784,12 +5259,12 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P20" si="0">SUM(F5:O5)</f>
+        <f t="shared" ref="P5:P21" si="0">SUM(F5:O5)</f>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="88"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="65" t="s">
         <v>72</v>
       </c>
@@ -4817,7 +5292,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="88"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="66" t="s">
         <v>73</v>
       </c>
@@ -4845,7 +5320,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="90"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="65" t="s">
         <v>74</v>
       </c>
@@ -4871,7 +5346,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="95" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="67" t="s">
@@ -4899,7 +5374,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="89"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="68" t="s">
         <v>89</v>
       </c>
@@ -4925,7 +5400,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="89"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="69" t="s">
         <v>75</v>
       </c>
@@ -4949,7 +5424,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="89"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="68" t="s">
         <v>76</v>
       </c>
@@ -4975,7 +5450,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="89"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="70" t="s">
         <v>77</v>
       </c>
@@ -5146,197 +5621,234 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="9"/>
+      <c r="P19" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="63"/>
-      <c r="C20" s="72" t="s">
-        <v>79</v>
+      <c r="B20" s="83"/>
+      <c r="C20" s="71" t="s">
+        <v>103</v>
       </c>
       <c r="D20" s="31"/>
-      <c r="E20" s="52">
-        <v>4</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="E20" s="53">
+        <v>3</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H20" s="4">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="20"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4">
+        <v>0.5</v>
+      </c>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="10">
+      <c r="P20" s="9">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="63"/>
+      <c r="C21" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="52">
+        <v>4</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
+        <v>4</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="86" t="s">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="23">
-        <f>SUM(E4:E20)</f>
-        <v>34.5</v>
-      </c>
-      <c r="F21" s="17">
-        <f t="shared" ref="F21:O21" si="2">E21-$E$21/10</f>
-        <v>31.05</v>
-      </c>
-      <c r="G21" s="17">
+      <c r="C22" s="92"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="23">
+        <f>SUM(E4:E21)</f>
+        <v>37.5</v>
+      </c>
+      <c r="F22" s="17">
+        <f t="shared" ref="F22:O22" si="2">E22-$E$22/10</f>
+        <v>33.75</v>
+      </c>
+      <c r="G22" s="17">
         <f t="shared" si="2"/>
-        <v>27.6</v>
-      </c>
-      <c r="H21" s="17">
+        <v>30</v>
+      </c>
+      <c r="H22" s="17">
         <f t="shared" si="2"/>
-        <v>24.150000000000002</v>
-      </c>
-      <c r="I21" s="17">
+        <v>26.25</v>
+      </c>
+      <c r="I22" s="17">
         <f t="shared" si="2"/>
-        <v>20.700000000000003</v>
-      </c>
-      <c r="J21" s="18">
+        <v>22.5</v>
+      </c>
+      <c r="J22" s="18">
         <f t="shared" si="2"/>
-        <v>17.250000000000004</v>
-      </c>
-      <c r="K21" s="17">
+        <v>18.75</v>
+      </c>
+      <c r="K22" s="17">
         <f t="shared" si="2"/>
-        <v>13.800000000000004</v>
-      </c>
-      <c r="L21" s="17">
+        <v>15</v>
+      </c>
+      <c r="L22" s="17">
         <f t="shared" si="2"/>
-        <v>10.350000000000005</v>
-      </c>
-      <c r="M21" s="17">
+        <v>11.25</v>
+      </c>
+      <c r="M22" s="17">
         <f t="shared" si="2"/>
-        <v>6.9000000000000048</v>
-      </c>
-      <c r="N21" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="N22" s="17">
         <f t="shared" si="2"/>
-        <v>3.4500000000000046</v>
-      </c>
-      <c r="O21" s="18">
+        <v>3.75</v>
+      </c>
+      <c r="O22" s="18">
         <f t="shared" si="2"/>
-        <v>4.4408920985006262E-15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="86" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="86"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="10">
-        <f>SUM(E4:E20)</f>
-        <v>34.5</v>
-      </c>
-      <c r="F22" s="6">
-        <f t="shared" ref="F22:O22" si="3">E22-(SUM(F4:F20))</f>
-        <v>27.5</v>
-      </c>
-      <c r="G22" s="6">
+      <c r="C23" s="92"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="10">
+        <f>SUM(E4:E21)</f>
+        <v>37.5</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" ref="F23:O23" si="3">E23-(SUM(F4:F21))</f>
+        <v>30</v>
+      </c>
+      <c r="G23" s="6">
         <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="H22" s="6">
+        <v>26</v>
+      </c>
+      <c r="H23" s="6">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="I22" s="6">
+        <v>15.5</v>
+      </c>
+      <c r="I23" s="6">
         <f t="shared" si="3"/>
-        <v>13.5</v>
-      </c>
-      <c r="J22" s="21">
+        <v>15</v>
+      </c>
+      <c r="J23" s="21">
         <f t="shared" si="3"/>
-        <v>13.5</v>
-      </c>
-      <c r="K22" s="6">
+        <v>15</v>
+      </c>
+      <c r="K23" s="6">
         <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-      <c r="L22" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="L23" s="6">
         <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-      <c r="M22" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="M23" s="6">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="N23" s="6">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="O22" s="7">
+        <v>0</v>
+      </c>
+      <c r="O23" s="7">
         <f t="shared" si="3"/>
-        <v>-0.5</v>
-      </c>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R23" s="65"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R24" s="66"/>
+      <c r="R24" s="65"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R25" s="65"/>
+      <c r="R25" s="66"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R26" s="66"/>
+      <c r="R26" s="65"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R27" s="65"/>
+      <c r="R27" s="66"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R28" s="66"/>
+      <c r="R28" s="65"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R29" s="65"/>
+      <c r="R29" s="66"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R30" s="66"/>
+      <c r="R30" s="65"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R31" s="65"/>
+      <c r="R31" s="66"/>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R32" s="66"/>
+      <c r="R32" s="65"/>
     </row>
     <row r="33" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R33" s="65"/>
+      <c r="R33" s="66"/>
     </row>
     <row r="34" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R34" s="66"/>
+      <c r="R34" s="65"/>
     </row>
     <row r="35" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R35" s="65"/>
+      <c r="R35" s="66"/>
     </row>
     <row r="36" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R36" s="66"/>
+      <c r="R36" s="65"/>
     </row>
     <row r="37" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R37" s="65"/>
+      <c r="R37" s="66"/>
+    </row>
+    <row r="38" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R38" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5348,8 +5860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF3C117-F50E-4201-8F00-39D353D27E11}">
   <dimension ref="B1:U32"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5371,34 +5883,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="83" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5476,7 +5988,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="93" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="66" t="s">
@@ -5504,7 +6016,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="88"/>
+      <c r="B6" s="94"/>
       <c r="C6" s="66" t="s">
         <v>95</v>
       </c>
@@ -5530,7 +6042,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="88"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="65" t="s">
         <v>96</v>
       </c>
@@ -5556,7 +6068,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="88"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="65" t="s">
         <v>98</v>
       </c>
@@ -5582,7 +6094,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="90"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="66" t="s">
         <v>97</v>
       </c>
@@ -5608,7 +6120,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="95" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="66" t="s">
@@ -5638,7 +6150,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="89"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="65" t="s">
         <v>92</v>
       </c>
@@ -5666,7 +6178,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="89"/>
+      <c r="B12" s="95"/>
       <c r="C12" s="65" t="s">
         <v>94</v>
       </c>
@@ -5728,140 +6240,124 @@
       <c r="I14" s="4"/>
       <c r="J14" s="20"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="L14" s="4">
+        <v>0.5</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="9"/>
+      <c r="P14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="76"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="65" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="60">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="4">
+        <v>0.5</v>
+      </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="4"/>
+      <c r="K15" s="4">
+        <v>0.5</v>
+      </c>
       <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4">
-        <v>4</v>
-      </c>
-      <c r="P15" s="10">
+      <c r="M15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="76"/>
+      <c r="C16" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="60">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4">
+        <v>2</v>
+      </c>
+      <c r="P16" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="86"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="23">
-        <f>SUM(E4:E15)</f>
-        <v>30.5</v>
-      </c>
-      <c r="F16" s="17">
-        <f t="shared" ref="F16:O16" si="1">E16-$E$16/10</f>
-        <v>27.45</v>
-      </c>
-      <c r="G16" s="17">
+      <c r="C17" s="98"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="23">
+        <f>SUM(E4:E16)</f>
+        <v>31.5</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" ref="F17:O17" si="1">E17-$E$17/10</f>
+        <v>28.35</v>
+      </c>
+      <c r="G17" s="17">
         <f t="shared" si="1"/>
-        <v>24.4</v>
-      </c>
-      <c r="H16" s="17">
+        <v>25.200000000000003</v>
+      </c>
+      <c r="H17" s="17">
         <f t="shared" si="1"/>
-        <v>21.349999999999998</v>
-      </c>
-      <c r="I16" s="17">
+        <v>22.050000000000004</v>
+      </c>
+      <c r="I17" s="17">
         <f t="shared" si="1"/>
-        <v>18.299999999999997</v>
-      </c>
-      <c r="J16" s="18">
+        <v>18.900000000000006</v>
+      </c>
+      <c r="J17" s="18">
         <f t="shared" si="1"/>
-        <v>15.249999999999996</v>
-      </c>
-      <c r="K16" s="17">
+        <v>15.750000000000005</v>
+      </c>
+      <c r="K17" s="17">
         <f t="shared" si="1"/>
-        <v>12.199999999999996</v>
-      </c>
-      <c r="L16" s="17">
+        <v>12.600000000000005</v>
+      </c>
+      <c r="L17" s="17">
         <f t="shared" si="1"/>
-        <v>9.149999999999995</v>
-      </c>
-      <c r="M16" s="17">
+        <v>9.4500000000000046</v>
+      </c>
+      <c r="M17" s="17">
         <f t="shared" si="1"/>
-        <v>6.0999999999999952</v>
-      </c>
-      <c r="N16" s="17">
+        <v>6.3000000000000043</v>
+      </c>
+      <c r="N17" s="17">
         <f t="shared" si="1"/>
-        <v>3.0499999999999954</v>
-      </c>
-      <c r="O16" s="18">
+        <v>3.1500000000000044</v>
+      </c>
+      <c r="O17" s="18">
         <f t="shared" si="1"/>
-        <v>-4.4408920985006262E-15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="10">
-        <f>SUM(E4:E15)</f>
-        <v>30.5</v>
-      </c>
-      <c r="F17" s="6">
-        <f t="shared" ref="F17:N17" si="2">E17-(SUM(F4:F15))</f>
-        <v>28.5</v>
-      </c>
-      <c r="G17" s="6">
-        <f t="shared" si="2"/>
-        <v>19.5</v>
-      </c>
-      <c r="H17" s="6">
-        <f t="shared" si="2"/>
-        <v>19.5</v>
-      </c>
-      <c r="I17" s="6">
-        <f t="shared" si="2"/>
-        <v>19.5</v>
-      </c>
-      <c r="J17" s="21">
-        <f t="shared" si="2"/>
-        <v>19.5</v>
-      </c>
-      <c r="K17" s="6">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
-      </c>
-      <c r="L17" s="6">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
-      </c>
-      <c r="M17" s="6">
-        <f t="shared" si="2"/>
-        <v>11.5</v>
-      </c>
-      <c r="N17" s="6">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
-      </c>
-      <c r="O17" s="7">
-        <f t="shared" ref="O17" si="3">N17-(SUM(O4:O12))</f>
-        <v>9.5</v>
-      </c>
-      <c r="P17" s="8"/>
+        <v>4.4408920985006262E-15</v>
+      </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -5869,6 +6365,56 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="98"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="10">
+        <f>SUM(E4:E16)</f>
+        <v>31.5</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" ref="F18:O18" si="2">E18-(SUM(F4:F16))</f>
+        <v>29.5</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J18" s="21">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="2"/>
+        <v>10.5</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O18" s="7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="P18" s="8"/>
       <c r="R18" s="65"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
@@ -5915,9 +6461,9 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
@@ -5932,10 +6478,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E11D258-16D5-404C-AFE4-ED632952B5DD}">
-  <dimension ref="B1:U28"/>
+  <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5957,34 +6503,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="84" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84" t="s">
+      <c r="C2" s="90" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="83" t="s">
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
     </row>
     <row r="3" spans="2:21" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -6036,7 +6582,7 @@
     <row r="4" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="81"/>
       <c r="C4" s="65" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="51">
@@ -6062,7 +6608,7 @@
     <row r="5" spans="2:21" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="79"/>
       <c r="C5" s="66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="58"/>
       <c r="E5" s="53">
@@ -6081,27 +6627,27 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P11" si="0">SUM(F5:O5)</f>
+        <f t="shared" ref="P5:P13" si="0">SUM(F5:O5)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="80"/>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="82"/>
       <c r="C6" s="66" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="31"/>
+        <v>107</v>
+      </c>
+      <c r="D6" s="58"/>
       <c r="E6" s="53">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
-        <v>2</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="20"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -6111,41 +6657,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="80"/>
-      <c r="C7" s="65" t="s">
-        <v>103</v>
+      <c r="C7" s="66" t="s">
+        <v>101</v>
       </c>
       <c r="D7" s="31"/>
-      <c r="E7" s="52">
+      <c r="E7" s="53">
         <v>2</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="20"/>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4">
+        <v>2</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="62">
+      <c r="P7" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="82"/>
-      <c r="C8" s="66" t="s">
-        <v>104</v>
+      <c r="C8" s="88" t="s">
+        <v>109</v>
       </c>
       <c r="D8" s="31"/>
-      <c r="E8" s="60">
-        <v>12</v>
+      <c r="E8" s="53">
+        <v>4</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>6</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="20"/>
@@ -6154,19 +6706,19 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="62">
+      <c r="P8" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="81"/>
-      <c r="C9" s="66" t="s">
-        <v>105</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="80"/>
+      <c r="C9" s="65" t="s">
+        <v>102</v>
       </c>
       <c r="D9" s="31"/>
-      <c r="E9" s="60">
-        <v>6</v>
+      <c r="E9" s="52">
+        <v>2</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -6183,14 +6735,555 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="81"/>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="60">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="4">
+        <v>3</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4">
+        <v>1</v>
+      </c>
+      <c r="O10" s="4">
+        <v>2</v>
+      </c>
+      <c r="P10" s="62">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="81"/>
+      <c r="C11" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="53">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4"/>
+      <c r="P11" s="62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="83"/>
+      <c r="C12" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="53">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="62">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="81"/>
+      <c r="C13" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="87">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="92"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="23">
+        <f>SUM(E4:E13)</f>
+        <v>24.5</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" ref="F14:O14" si="1">E14-$E$14/10</f>
+        <v>22.05</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="1"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H14" s="17">
+        <f t="shared" si="1"/>
+        <v>17.150000000000002</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="1"/>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="1"/>
+        <v>12.250000000000004</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="1"/>
+        <v>9.8000000000000043</v>
+      </c>
+      <c r="L14" s="17">
+        <f t="shared" si="1"/>
+        <v>7.3500000000000041</v>
+      </c>
+      <c r="M14" s="17">
+        <f t="shared" si="1"/>
+        <v>4.9000000000000039</v>
+      </c>
+      <c r="N14" s="17">
+        <f t="shared" si="1"/>
+        <v>2.4500000000000037</v>
+      </c>
+      <c r="O14" s="18">
+        <f t="shared" si="1"/>
+        <v>3.5527136788005009E-15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="92"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="10">
+        <f>SUM(E4:E13)</f>
+        <v>24.5</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" ref="F15:O15" si="2">E15-(SUM(F4:F13))</f>
+        <v>21.5</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="J15" s="21">
+        <f t="shared" si="2"/>
+        <v>15.5</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O15" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R16" s="65"/>
+    </row>
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="66"/>
+    </row>
+    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="65"/>
+    </row>
+    <row r="19" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R19" s="66"/>
+    </row>
+    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="65"/>
+    </row>
+    <row r="21" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R21" s="66"/>
+    </row>
+    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R22" s="65"/>
+    </row>
+    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="66"/>
+    </row>
+    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="65"/>
+    </row>
+    <row r="25" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="66"/>
+    </row>
+    <row r="26" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="65"/>
+    </row>
+    <row r="27" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="66"/>
+    </row>
+    <row r="28" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R28" s="65"/>
+    </row>
+    <row r="29" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="66"/>
+    </row>
+    <row r="30" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R30" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E818FB47-CBCC-493F-B743-7459456B11F1}">
+  <dimension ref="B1:U29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="7" width="7.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="7" style="5" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7.625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="5.875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="90" t="s">
         <v>106</v>
+      </c>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="89" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+    </row>
+    <row r="3" spans="2:21" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="86"/>
+      <c r="C4" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="23">
+        <f>SUM(F4:O4)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="84"/>
+      <c r="C5" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="9">
+        <f t="shared" ref="P5:P12" si="0">SUM(F5:O5)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="85"/>
+      <c r="C6" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="53">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="85"/>
+      <c r="C7" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="53">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="85"/>
+      <c r="C8" s="88" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="53">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="85"/>
+      <c r="C9" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="52">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="86"/>
+      <c r="C10" s="88" t="s">
+        <v>113</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="53">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -6208,192 +7301,215 @@
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="81"/>
-      <c r="C11" s="65" t="s">
-        <v>61</v>
+      <c r="B11" s="86"/>
+      <c r="C11" s="88" t="s">
+        <v>116</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="52">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="E11" s="53">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="20"/>
-      <c r="K11" s="4"/>
+      <c r="K11" s="4">
+        <v>3</v>
+      </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="62">
+      <c r="P11" s="62"/>
+    </row>
+    <row r="12" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="86"/>
+      <c r="C12" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="52">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="4">
+        <v>2</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="87">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="23">
-        <f>SUM(E4:E11)</f>
-        <v>27.5</v>
-      </c>
-      <c r="F12" s="17">
-        <f t="shared" ref="F12:O12" si="1">E12-$E$12/10</f>
-        <v>24.75</v>
-      </c>
-      <c r="G12" s="17">
+      <c r="C13" s="92"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="23">
+        <f>SUM(E4:E12)</f>
+        <v>29.5</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" ref="F13:O13" si="1">E13-$E$13/10</f>
+        <v>26.55</v>
+      </c>
+      <c r="G13" s="17">
         <f t="shared" si="1"/>
+        <v>23.6</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" si="1"/>
+        <v>20.650000000000002</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="1"/>
+        <v>17.700000000000003</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" si="1"/>
+        <v>14.750000000000004</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="1"/>
+        <v>11.800000000000004</v>
+      </c>
+      <c r="L13" s="17">
+        <f t="shared" si="1"/>
+        <v>8.850000000000005</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="1"/>
+        <v>5.9000000000000048</v>
+      </c>
+      <c r="N13" s="17">
+        <f t="shared" si="1"/>
+        <v>2.9500000000000046</v>
+      </c>
+      <c r="O13" s="18">
+        <f t="shared" si="1"/>
+        <v>4.4408920985006262E-15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="92"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="10">
+        <f>SUM(E4:E12)</f>
+        <v>29.5</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14:O14" si="2">E14-(SUM(F4:F12))</f>
         <v>22</v>
       </c>
-      <c r="H12" s="17">
-        <f t="shared" si="1"/>
-        <v>19.25</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="1"/>
-        <v>16.5</v>
-      </c>
-      <c r="J12" s="18">
-        <f t="shared" si="1"/>
-        <v>13.75</v>
-      </c>
-      <c r="K12" s="17">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="L12" s="17">
-        <f t="shared" si="1"/>
-        <v>8.25</v>
-      </c>
-      <c r="M12" s="17">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-      <c r="N12" s="17">
-        <f t="shared" si="1"/>
-        <v>2.75</v>
-      </c>
-      <c r="O12" s="18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="10">
-        <f>SUM(E4:E11)</f>
-        <v>27.5</v>
-      </c>
-      <c r="F13" s="6">
-        <f>E13-(SUM(F4:F11))</f>
-        <v>25</v>
-      </c>
-      <c r="G13" s="6">
-        <f>F13-(SUM(G4:G11))</f>
-        <v>25</v>
-      </c>
-      <c r="H13" s="6">
-        <f>G13-(SUM(H4:H11))</f>
-        <v>25</v>
-      </c>
-      <c r="I13" s="6">
-        <f>H13-(SUM(I4:I11))</f>
-        <v>25</v>
-      </c>
-      <c r="J13" s="21">
-        <f>I13-(SUM(J4:J11))</f>
-        <v>25</v>
-      </c>
-      <c r="K13" s="6">
-        <f>J13-(SUM(K4:K11))</f>
-        <v>21</v>
-      </c>
-      <c r="L13" s="6">
-        <f>K13-(SUM(L4:L11))</f>
-        <v>21</v>
-      </c>
-      <c r="M13" s="6">
-        <f>L13-(SUM(M4:M11))</f>
-        <v>21</v>
-      </c>
-      <c r="N13" s="6">
-        <f>M13-(SUM(N4:N11))</f>
-        <v>21</v>
-      </c>
-      <c r="O13" s="7">
-        <f>N13-(SUM(O4:O11))</f>
-        <v>21</v>
-      </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R14" s="65"/>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="J14" s="21">
+        <f t="shared" si="2"/>
+        <v>21.5</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R15" s="66"/>
+      <c r="R15" s="65"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R16" s="65"/>
+      <c r="R16" s="66"/>
     </row>
     <row r="17" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R17" s="66"/>
+      <c r="R17" s="65"/>
     </row>
     <row r="18" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R18" s="65"/>
+      <c r="R18" s="66"/>
     </row>
     <row r="19" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R19" s="66"/>
+      <c r="R19" s="65"/>
     </row>
     <row r="20" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R20" s="65"/>
+      <c r="R20" s="66"/>
     </row>
     <row r="21" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R21" s="66"/>
+      <c r="R21" s="65"/>
     </row>
     <row r="22" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R22" s="65"/>
+      <c r="R22" s="66"/>
     </row>
     <row r="23" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R23" s="66"/>
+      <c r="R23" s="65"/>
     </row>
     <row r="24" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R24" s="65"/>
+      <c r="R24" s="66"/>
     </row>
     <row r="25" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R25" s="66"/>
+      <c r="R25" s="65"/>
     </row>
     <row r="26" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R26" s="65"/>
+      <c r="R26" s="66"/>
     </row>
     <row r="27" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R27" s="66"/>
+      <c r="R27" s="65"/>
     </row>
     <row r="28" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R28" s="65"/>
+      <c r="R28" s="66"/>
+    </row>
+    <row r="29" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6401,7 +7517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:W18"/>
   <sheetViews>
@@ -6430,38 +7546,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="83" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -6517,7 +7633,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="93" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -6571,7 +7687,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="90"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -6623,7 +7739,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="93" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -6669,7 +7785,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="88"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -6713,7 +7829,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="88"/>
+      <c r="B8" s="94"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -6757,7 +7873,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="88"/>
+      <c r="B9" s="94"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -6801,7 +7917,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="88"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -6845,7 +7961,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="88"/>
+      <c r="B11" s="94"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -6889,7 +8005,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="88"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -6933,7 +8049,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="88"/>
+      <c r="B13" s="94"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -6977,7 +8093,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="88"/>
+      <c r="B14" s="94"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -7021,7 +8137,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="88"/>
+      <c r="B15" s="94"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -7065,7 +8181,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="90"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -7109,11 +8225,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -7162,11 +8278,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">

</xml_diff>

<commit_message>
added test scripts for access testing to git *** this is ahead of deployed version due to hold up with questionairs DO NOT DEPLOY
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5E3F5E-2042-4917-8B33-FC10E0540A5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9B478F-1C39-4532-AE12-C7776F23E024}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29715" yWindow="1020" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1095" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -2679,37 +2679,37 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>29.5</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.55</c:v>
+                  <c:v>27.45</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.6</c:v>
+                  <c:v>24.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.650000000000002</c:v>
+                  <c:v>21.349999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.700000000000003</c:v>
+                  <c:v>18.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.750000000000004</c:v>
+                  <c:v>15.249999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.800000000000004</c:v>
+                  <c:v>12.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.850000000000005</c:v>
+                  <c:v>9.149999999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.9000000000000048</c:v>
+                  <c:v>6.0999999999999952</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9500000000000046</c:v>
+                  <c:v>3.0499999999999954</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4408920985006262E-15</c:v>
+                  <c:v>-4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2778,7 +2778,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>29.5</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>22</c:v>
@@ -2796,19 +2796,19 @@
                   <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5841,14 +5841,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6461,14 +6461,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B5:B9"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6480,7 +6480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E11D258-16D5-404C-AFE4-ED632952B5DD}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -7019,8 +7019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E818FB47-CBCC-493F-B743-7459456B11F1}">
   <dimension ref="B1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7259,21 +7259,27 @@
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="52">
-        <v>2</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="20"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
@@ -7291,13 +7297,15 @@
       <c r="I10" s="4"/>
       <c r="J10" s="20"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="L10" s="5">
+        <v>2</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
@@ -7317,13 +7325,16 @@
       <c r="K11" s="4">
         <v>3</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="L11" s="4">
         <v>1</v>
       </c>
+      <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="62"/>
+      <c r="P11" s="62">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="2:21" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="86"/>
@@ -7359,47 +7370,47 @@
       <c r="D13" s="32"/>
       <c r="E13" s="23">
         <f>SUM(E4:E12)</f>
-        <v>29.5</v>
+        <v>30.5</v>
       </c>
       <c r="F13" s="17">
         <f t="shared" ref="F13:O13" si="1">E13-$E$13/10</f>
-        <v>26.55</v>
+        <v>27.45</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="1"/>
-        <v>23.6</v>
+        <v>24.4</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" si="1"/>
-        <v>20.650000000000002</v>
+        <v>21.349999999999998</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" si="1"/>
-        <v>17.700000000000003</v>
+        <v>18.299999999999997</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="1"/>
-        <v>14.750000000000004</v>
+        <v>15.249999999999996</v>
       </c>
       <c r="K13" s="17">
         <f t="shared" si="1"/>
-        <v>11.800000000000004</v>
+        <v>12.199999999999996</v>
       </c>
       <c r="L13" s="17">
         <f t="shared" si="1"/>
-        <v>8.850000000000005</v>
+        <v>9.149999999999995</v>
       </c>
       <c r="M13" s="17">
         <f t="shared" si="1"/>
-        <v>5.9000000000000048</v>
+        <v>6.0999999999999952</v>
       </c>
       <c r="N13" s="17">
         <f t="shared" si="1"/>
-        <v>2.9500000000000046</v>
+        <v>3.0499999999999954</v>
       </c>
       <c r="O13" s="18">
         <f t="shared" si="1"/>
-        <v>4.4408920985006262E-15</v>
+        <v>-4.4408920985006262E-15</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
@@ -7410,7 +7421,7 @@
       <c r="D14" s="33"/>
       <c r="E14" s="10">
         <f>SUM(E4:E12)</f>
-        <v>29.5</v>
+        <v>30.5</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" ref="F14:O14" si="2">E14-(SUM(F4:F12))</f>
@@ -7434,23 +7445,23 @@
       </c>
       <c r="K14" s="6">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>12.5</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>7.5</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>7.5</v>
       </c>
       <c r="N14" s="6">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>7.5</v>
       </c>
       <c r="O14" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>7.5</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="2"/>
@@ -8340,14 +8351,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added requirement icons added styling to tasks addeddeadline date *** this is ahead of deployed version due to hold up with questionairs DO NOT DEPLOY
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9B478F-1C39-4532-AE12-C7776F23E024}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D361F-3A91-44FD-A269-8DC35BEC9DE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1095" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29475" yWindow="1920" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Sprint Backlog 3" sheetId="7" r:id="rId4"/>
     <sheet name="Sprint Backlog 4" sheetId="8" r:id="rId5"/>
     <sheet name="Sprint Backlog 5" sheetId="9" r:id="rId6"/>
-    <sheet name="Sprint Backlog example" sheetId="4" r:id="rId7"/>
+    <sheet name="Sprint Backlog 6" sheetId="10" r:id="rId7"/>
+    <sheet name="Sprint Backlog example" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="126">
   <si>
     <t>Task</t>
   </si>
@@ -427,6 +428,30 @@
   </si>
   <si>
     <t>Information Arechecture</t>
+  </si>
+  <si>
+    <t>Conduct remaining surveys</t>
+  </si>
+  <si>
+    <t>Deadline display</t>
+  </si>
+  <si>
+    <t>User access tests</t>
+  </si>
+  <si>
+    <t>Teams access tests</t>
+  </si>
+  <si>
+    <t>Tasks access tests</t>
+  </si>
+  <si>
+    <t>Team types access</t>
+  </si>
+  <si>
+    <t>06/01/2020-20/01/2020</t>
+  </si>
+  <si>
+    <t>20/01/2020-02/02/2020</t>
   </si>
 </sst>
 </file>
@@ -905,7 +930,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1151,6 +1176,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2927,6 +2961,340 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16282253282832151"/>
+          <c:y val="1.8470584658792262E-2"/>
+          <c:w val="0.71469100453352397"/>
+          <c:h val="0.79831147760594201"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 6'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 6'!$E$13:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.050000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.750000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4500000000000046</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3000000000000043</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1500000000000044</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.4408920985006262E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF84-4FEB-AA0A-A632B1DB7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Effort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint Backlog 6'!$E$3:$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Estimate Effort hours</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fri</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mon</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tues</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Wed</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Thur</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Fri</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog 6'!$E$14:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BF84-4FEB-AA0A-A632B1DB7345}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="132299304"/>
+        <c:axId val="132299696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="132299304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DAYS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="132299696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>HOURS EFFORT</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132299304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3474,6 +3842,49 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>475111</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>131724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>252860</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>121138</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{692E174B-415B-417D-87DD-AF548682E473}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4246,34 +4657,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="89" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4323,7 +4734,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="98" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="54" t="s">
@@ -4369,7 +4780,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="95"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="57" t="s">
         <v>65</v>
       </c>
@@ -4413,7 +4824,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="95"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="56" t="s">
         <v>61</v>
       </c>
@@ -4457,7 +4868,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="95"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="55"/>
       <c r="D7" s="31"/>
       <c r="E7" s="52"/>
@@ -4497,7 +4908,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="96" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="61" t="s">
@@ -4543,7 +4954,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="94"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="57" t="s">
         <v>67</v>
       </c>
@@ -4587,7 +4998,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="94"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="59" t="s">
         <v>60</v>
       </c>
@@ -4631,7 +5042,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="94"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="56" t="s">
         <v>57</v>
       </c>
@@ -4675,7 +5086,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="94"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="54" t="s">
         <v>58</v>
       </c>
@@ -4719,7 +5130,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="94"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="54" t="s">
         <v>69</v>
       </c>
@@ -4763,7 +5174,7 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="94"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="54" t="s">
         <v>68</v>
       </c>
@@ -4805,7 +5216,7 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="96"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="56" t="s">
         <v>59</v>
       </c>
@@ -4889,7 +5300,7 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="93" t="s">
+      <c r="B17" s="96" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="54" t="s">
@@ -4935,7 +5346,7 @@
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="94"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="54" t="s">
         <v>63</v>
       </c>
@@ -4979,10 +5390,10 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="92"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="32"/>
       <c r="E19" s="23">
         <f>SUM(E4:E18)</f>
@@ -5030,10 +5441,10 @@
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="92"/>
+      <c r="C20" s="95"/>
       <c r="D20" s="33"/>
       <c r="E20" s="10">
         <f>SUM(E4:E18)</f>
@@ -5131,34 +5542,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="89" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5236,7 +5647,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="96" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="73" t="s">
@@ -5264,7 +5675,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="94"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="65" t="s">
         <v>72</v>
       </c>
@@ -5292,7 +5703,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="94"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="66" t="s">
         <v>73</v>
       </c>
@@ -5320,7 +5731,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="96"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="65" t="s">
         <v>74</v>
       </c>
@@ -5346,7 +5757,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="98" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="67" t="s">
@@ -5374,7 +5785,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="95"/>
+      <c r="B10" s="98"/>
       <c r="C10" s="68" t="s">
         <v>89</v>
       </c>
@@ -5400,7 +5811,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="69" t="s">
         <v>75</v>
       </c>
@@ -5424,7 +5835,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="95"/>
+      <c r="B12" s="98"/>
       <c r="C12" s="68" t="s">
         <v>76</v>
       </c>
@@ -5450,7 +5861,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="95"/>
+      <c r="B13" s="98"/>
       <c r="C13" s="70" t="s">
         <v>77</v>
       </c>
@@ -5687,10 +6098,10 @@
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="92"/>
+      <c r="C22" s="95"/>
       <c r="D22" s="32"/>
       <c r="E22" s="23">
         <f>SUM(E4:E21)</f>
@@ -5738,10 +6149,10 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="92"/>
+      <c r="C23" s="95"/>
       <c r="D23" s="33"/>
       <c r="E23" s="10">
         <f>SUM(E4:E21)</f>
@@ -5841,14 +6252,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5883,34 +6294,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="89" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5988,7 +6399,7 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="96" t="s">
         <v>82</v>
       </c>
       <c r="C5" s="66" t="s">
@@ -6016,7 +6427,7 @@
       </c>
     </row>
     <row r="6" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="94"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="66" t="s">
         <v>95</v>
       </c>
@@ -6042,7 +6453,7 @@
       </c>
     </row>
     <row r="7" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="94"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="65" t="s">
         <v>96</v>
       </c>
@@ -6068,7 +6479,7 @@
       </c>
     </row>
     <row r="8" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="94"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="65" t="s">
         <v>98</v>
       </c>
@@ -6094,7 +6505,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="96"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="66" t="s">
         <v>97</v>
       </c>
@@ -6120,7 +6531,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="98" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="66" t="s">
@@ -6150,7 +6561,7 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="65" t="s">
         <v>92</v>
       </c>
@@ -6178,7 +6589,7 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="95"/>
+      <c r="B12" s="98"/>
       <c r="C12" s="65" t="s">
         <v>94</v>
       </c>
@@ -6309,10 +6720,10 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="98"/>
+      <c r="C17" s="101"/>
       <c r="D17" s="32"/>
       <c r="E17" s="23">
         <f>SUM(E4:E16)</f>
@@ -6365,10 +6776,10 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="98"/>
+      <c r="C18" s="101"/>
       <c r="D18" s="33"/>
       <c r="E18" s="10">
         <f>SUM(E4:E16)</f>
@@ -6461,14 +6872,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B10:B12"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B5:B9"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6480,8 +6891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E11D258-16D5-404C-AFE4-ED632952B5DD}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6503,34 +6914,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="89" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="2:21" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -6848,10 +7259,10 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="92"/>
+      <c r="C14" s="95"/>
       <c r="D14" s="32"/>
       <c r="E14" s="23">
         <f>SUM(E4:E13)</f>
@@ -6899,10 +7310,10 @@
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="92"/>
+      <c r="C15" s="95"/>
       <c r="D15" s="33"/>
       <c r="E15" s="10">
         <f>SUM(E4:E13)</f>
@@ -7019,8 +7430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E818FB47-CBCC-493F-B743-7459456B11F1}">
   <dimension ref="B1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7042,34 +7453,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="90" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90" t="s">
+      <c r="C2" s="93" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="89" t="s">
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="2:21" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -7363,10 +7774,10 @@
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="92"/>
+      <c r="C13" s="95"/>
       <c r="D13" s="32"/>
       <c r="E13" s="23">
         <f>SUM(E4:E12)</f>
@@ -7414,10 +7825,10 @@
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="92"/>
+      <c r="C14" s="95"/>
       <c r="D14" s="33"/>
       <c r="E14" s="10">
         <f>SUM(E4:E12)</f>
@@ -7531,6 +7942,490 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE7B8EB-21C0-4CBB-8AEE-47C844F862DC}">
+  <dimension ref="B1:U29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="7.375" style="5" customWidth="1"/>
+    <col min="6" max="7" width="7.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="6.875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="7" style="5" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="7.625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="7.375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="7.625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="5.875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="92" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+    </row>
+    <row r="3" spans="2:21" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="91"/>
+      <c r="C4" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="23">
+        <f>SUM(F4:O4)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="89"/>
+      <c r="C5" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="9">
+        <f t="shared" ref="P5:P12" si="0">SUM(F5:O5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="90"/>
+      <c r="C6" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="53">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="90"/>
+      <c r="C7" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="53">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="90"/>
+      <c r="C8" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="53">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="90"/>
+      <c r="C9" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="52">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="91"/>
+      <c r="C10" s="88" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="53">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="91"/>
+      <c r="C11" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="53">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="91"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="95"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="23">
+        <f>SUM(E4:E12)</f>
+        <v>31.5</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" ref="F13:O13" si="1">E13-$E$13/10</f>
+        <v>28.35</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="1"/>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" si="1"/>
+        <v>22.050000000000004</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="1"/>
+        <v>18.900000000000006</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" si="1"/>
+        <v>15.750000000000005</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="1"/>
+        <v>12.600000000000005</v>
+      </c>
+      <c r="L13" s="17">
+        <f t="shared" si="1"/>
+        <v>9.4500000000000046</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="1"/>
+        <v>6.3000000000000043</v>
+      </c>
+      <c r="N13" s="17">
+        <f t="shared" si="1"/>
+        <v>3.1500000000000044</v>
+      </c>
+      <c r="O13" s="18">
+        <f t="shared" si="1"/>
+        <v>4.4408920985006262E-15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="95"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="10">
+        <f>SUM(E4:E12)</f>
+        <v>31.5</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14:O14" si="2">E14-(SUM(F4:F12))</f>
+        <v>31</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="J14" s="21">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R15" s="65"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R16" s="66"/>
+    </row>
+    <row r="17" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="65"/>
+    </row>
+    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="66"/>
+    </row>
+    <row r="19" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R19" s="65"/>
+    </row>
+    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="66"/>
+    </row>
+    <row r="21" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R21" s="65"/>
+    </row>
+    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R22" s="66"/>
+    </row>
+    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="65"/>
+    </row>
+    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="66"/>
+    </row>
+    <row r="25" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="65"/>
+    </row>
+    <row r="26" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="66"/>
+    </row>
+    <row r="27" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="65"/>
+    </row>
+    <row r="28" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R28" s="66"/>
+    </row>
+    <row r="29" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R29" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:W18"/>
   <sheetViews>
@@ -7559,38 +8454,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="89" t="s">
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
     </row>
     <row r="3" spans="2:18" s="3" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -7646,7 +8541,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="96" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -7700,7 +8595,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="96"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
@@ -7752,7 +8647,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="96" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="16"/>
@@ -7798,7 +8693,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="94"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="31"/>
@@ -7842,7 +8737,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="94"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="31"/>
@@ -7886,7 +8781,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="94"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="31"/>
@@ -7930,7 +8825,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="94"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="31"/>
@@ -7974,7 +8869,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="94"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="31"/>
@@ -8018,7 +8913,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="94"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="31"/>
@@ -8062,7 +8957,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="94"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="31"/>
@@ -8106,7 +9001,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="94"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="31"/>
@@ -8150,7 +9045,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="94"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="31"/>
@@ -8194,7 +9089,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="96"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="31"/>
@@ -8238,11 +9133,11 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="92"/>
-      <c r="D17" s="92"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -8291,11 +9186,11 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="92"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="G18" s="10">
@@ -8351,14 +9246,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
applying documentation changes to git refactored requirement and reward tiles lists into there own custom element this cleans up task cards somewhat
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D361F-3A91-44FD-A269-8DC35BEC9DE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EC97AB-22B8-433E-A760-0960140A125F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29475" yWindow="1920" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="127">
   <si>
     <t>Task</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>20/01/2020-02/02/2020</t>
+  </si>
+  <si>
+    <t>Requirements Display</t>
   </si>
 </sst>
 </file>
@@ -3042,39 +3045,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 6'!$E$13:$O$13</c:f>
+              <c:f>'Sprint Backlog 6'!$E$14:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>31.5</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.35</c:v>
+                  <c:v>31.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.200000000000003</c:v>
+                  <c:v>27.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.050000000000004</c:v>
+                  <c:v>24.150000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.900000000000006</c:v>
+                  <c:v>20.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.750000000000005</c:v>
+                  <c:v>17.250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.600000000000005</c:v>
+                  <c:v>13.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.4500000000000046</c:v>
+                  <c:v>10.350000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.3000000000000043</c:v>
+                  <c:v>6.9000000000000048</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1500000000000044</c:v>
+                  <c:v>3.4500000000000046</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4.4408920985006262E-15</c:v>
@@ -3141,42 +3144,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint Backlog 6'!$E$14:$O$14</c:f>
+              <c:f>'Sprint Backlog 6'!$E$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>31.5</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3847,13 +3850,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>475111</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>131724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>252860</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>121138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7943,10 +7946,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE7B8EB-21C0-4CBB-8AEE-47C844F862DC}">
-  <dimension ref="B1:U29"/>
+  <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8090,42 +8093,43 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="9">
-        <f t="shared" ref="P5:P12" si="0">SUM(F5:O5)</f>
+        <f t="shared" ref="P5:P13" si="0">SUM(F5:O5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="90"/>
       <c r="C6" s="66" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D6" s="58"/>
       <c r="E6" s="53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="20"/>
+      <c r="J6" s="20">
+        <v>1</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="90"/>
       <c r="C7" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="31"/>
+        <v>119</v>
+      </c>
+      <c r="D7" s="58"/>
       <c r="E7" s="53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -8144,15 +8148,17 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="90"/>
-      <c r="C8" s="88" t="s">
-        <v>121</v>
+      <c r="C8" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="53">
         <v>5</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="20"/>
@@ -8163,21 +8169,25 @@
       <c r="O8" s="4"/>
       <c r="P8" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="90"/>
-      <c r="C9" s="65" t="s">
-        <v>122</v>
+      <c r="C9" s="88" t="s">
+        <v>121</v>
       </c>
       <c r="D9" s="31"/>
-      <c r="E9" s="52">
+      <c r="E9" s="53">
         <v>5</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="20"/>
       <c r="K9" s="4"/>
@@ -8185,42 +8195,45 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="62">
+      <c r="P9" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="91"/>
-      <c r="C10" s="88" t="s">
-        <v>123</v>
+      <c r="B10" s="90"/>
+      <c r="C10" s="65" t="s">
+        <v>122</v>
       </c>
       <c r="D10" s="31"/>
-      <c r="E10" s="53">
-        <v>6</v>
+      <c r="E10" s="52">
+        <v>5</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4">
+        <v>2</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="20"/>
       <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="91"/>
       <c r="C11" s="88" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="53">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -8228,7 +8241,6 @@
       <c r="I11" s="4"/>
       <c r="J11" s="20"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -8239,12 +8251,22 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="91"/>
-      <c r="C12" s="88"/>
+      <c r="C12" s="88" t="s">
+        <v>103</v>
+      </c>
       <c r="D12" s="31"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="E12" s="53">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.5</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="20"/>
       <c r="K12" s="4"/>
@@ -8252,163 +8274,183 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="87">
+      <c r="P12" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="91"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="87">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="23">
-        <f>SUM(E4:E12)</f>
-        <v>31.5</v>
-      </c>
-      <c r="F13" s="17">
-        <f t="shared" ref="F13:O13" si="1">E13-$E$13/10</f>
-        <v>28.35</v>
-      </c>
-      <c r="G13" s="17">
+      <c r="C14" s="95"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="23">
+        <f>SUM(E4:E13)</f>
+        <v>34.5</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" ref="F14:O14" si="1">E14-$E$14/10</f>
+        <v>31.05</v>
+      </c>
+      <c r="G14" s="17">
         <f t="shared" si="1"/>
-        <v>25.200000000000003</v>
-      </c>
-      <c r="H13" s="17">
+        <v>27.6</v>
+      </c>
+      <c r="H14" s="17">
         <f t="shared" si="1"/>
-        <v>22.050000000000004</v>
-      </c>
-      <c r="I13" s="17">
+        <v>24.150000000000002</v>
+      </c>
+      <c r="I14" s="17">
         <f t="shared" si="1"/>
-        <v>18.900000000000006</v>
-      </c>
-      <c r="J13" s="18">
+        <v>20.700000000000003</v>
+      </c>
+      <c r="J14" s="18">
         <f t="shared" si="1"/>
-        <v>15.750000000000005</v>
-      </c>
-      <c r="K13" s="17">
+        <v>17.250000000000004</v>
+      </c>
+      <c r="K14" s="17">
         <f t="shared" si="1"/>
-        <v>12.600000000000005</v>
-      </c>
-      <c r="L13" s="17">
+        <v>13.800000000000004</v>
+      </c>
+      <c r="L14" s="17">
         <f t="shared" si="1"/>
-        <v>9.4500000000000046</v>
-      </c>
-      <c r="M13" s="17">
+        <v>10.350000000000005</v>
+      </c>
+      <c r="M14" s="17">
         <f t="shared" si="1"/>
-        <v>6.3000000000000043</v>
-      </c>
-      <c r="N13" s="17">
+        <v>6.9000000000000048</v>
+      </c>
+      <c r="N14" s="17">
         <f t="shared" si="1"/>
-        <v>3.1500000000000044</v>
-      </c>
-      <c r="O13" s="18">
+        <v>3.4500000000000046</v>
+      </c>
+      <c r="O14" s="18">
         <f t="shared" si="1"/>
         <v>4.4408920985006262E-15</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="95" t="s">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="95"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="10">
-        <f>SUM(E4:E12)</f>
-        <v>31.5</v>
-      </c>
-      <c r="F14" s="6">
-        <f t="shared" ref="F14:O14" si="2">E14-(SUM(F4:F12))</f>
-        <v>31</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="C15" s="95"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="10">
+        <f>SUM(E4:E13)</f>
+        <v>34.5</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" ref="F15:O15" si="2">E15-(SUM(F4:F13))</f>
+        <v>33.5</v>
+      </c>
+      <c r="G15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="H14" s="6">
+        <v>28</v>
+      </c>
+      <c r="H15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="I14" s="6">
+        <v>22.5</v>
+      </c>
+      <c r="I15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="J14" s="21">
+        <v>22.5</v>
+      </c>
+      <c r="J15" s="21">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="K14" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="K15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="L14" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="L15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="M14" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="N14" s="6">
+        <v>21.5</v>
+      </c>
+      <c r="N15" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="O14" s="7">
+        <v>21.5</v>
+      </c>
+      <c r="O15" s="7">
         <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R15" s="65"/>
+        <v>21.5</v>
+      </c>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R16" s="66"/>
+      <c r="R16" s="65"/>
     </row>
     <row r="17" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R17" s="65"/>
+      <c r="R17" s="66"/>
     </row>
     <row r="18" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R18" s="66"/>
+      <c r="R18" s="65"/>
     </row>
     <row r="19" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R19" s="65"/>
+      <c r="R19" s="66"/>
     </row>
     <row r="20" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R20" s="66"/>
+      <c r="R20" s="65"/>
     </row>
     <row r="21" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R21" s="65"/>
+      <c r="R21" s="66"/>
     </row>
     <row r="22" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R22" s="66"/>
+      <c r="R22" s="65"/>
     </row>
     <row r="23" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R23" s="65"/>
+      <c r="R23" s="66"/>
     </row>
     <row r="24" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R24" s="66"/>
+      <c r="R24" s="65"/>
     </row>
     <row r="25" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R25" s="65"/>
+      <c r="R25" s="66"/>
     </row>
     <row r="26" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R26" s="66"/>
+      <c r="R26" s="65"/>
     </row>
     <row r="27" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R27" s="65"/>
+      <c r="R27" s="66"/>
     </row>
     <row r="28" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R28" s="66"/>
+      <c r="R28" s="65"/>
     </row>
     <row r="29" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R29" s="65"/>
+      <c r="R29" s="66"/>
+    </row>
+    <row r="30" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R30" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8416,8 +8458,8 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
fixed issue with safari compatibility, option parameter is unsupported custom extensions of existing elements not possible
</commit_message>
<xml_diff>
--- a/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
+++ b/Planning Report/projectscrumburndownchart- jordan harrison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\CI301-repo\CI301\Planning Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EC97AB-22B8-433E-A760-0960140A125F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804D3BCD-B57A-4363-8C71-103A51DAF46D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29475" yWindow="1920" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24345" windowHeight="14040" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -3050,37 +3050,37 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>34.5</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.05</c:v>
+                  <c:v>25.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.6</c:v>
+                  <c:v>22.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.150000000000002</c:v>
+                  <c:v>19.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.700000000000003</c:v>
+                  <c:v>17.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.250000000000004</c:v>
+                  <c:v>14.249999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.800000000000004</c:v>
+                  <c:v>11.399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.350000000000005</c:v>
+                  <c:v>8.5499999999999954</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9000000000000048</c:v>
+                  <c:v>5.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4500000000000046</c:v>
+                  <c:v>2.8499999999999956</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.4408920985006262E-15</c:v>
+                  <c:v>-4.4408920985006262E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3149,37 +3149,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>34.5</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.5</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.5</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6255,14 +6255,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6875,14 +6875,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B10:B12"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B5:B9"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7433,8 +7433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E818FB47-CBCC-493F-B743-7459456B11F1}">
   <dimension ref="B1:U29"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7948,8 +7948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE7B8EB-21C0-4CBB-8AEE-47C844F862DC}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8087,14 +8087,18 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="4"/>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="O5" s="4">
+        <v>2</v>
+      </c>
       <c r="P5" s="9">
         <f t="shared" ref="P5:P13" si="0">SUM(F5:O5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
@@ -8116,11 +8120,16 @@
         <v>1</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4">
+        <v>2</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="9"/>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="90"/>
@@ -8129,13 +8138,15 @@
       </c>
       <c r="D7" s="58"/>
       <c r="E7" s="53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="20"/>
+      <c r="J7" s="20">
+        <v>1</v>
+      </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -8143,7 +8154,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
@@ -8233,20 +8244,22 @@
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="53">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="20"/>
+      <c r="J11" s="20">
+        <v>3</v>
+      </c>
       <c r="K11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
@@ -8268,15 +8281,18 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="J12" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.5</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="62">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
@@ -8307,47 +8323,47 @@
       <c r="D14" s="32"/>
       <c r="E14" s="23">
         <f>SUM(E4:E13)</f>
-        <v>34.5</v>
+        <v>28.5</v>
       </c>
       <c r="F14" s="17">
         <f t="shared" ref="F14:O14" si="1">E14-$E$14/10</f>
-        <v>31.05</v>
+        <v>25.65</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" si="1"/>
-        <v>27.6</v>
+        <v>22.799999999999997</v>
       </c>
       <c r="H14" s="17">
         <f t="shared" si="1"/>
-        <v>24.150000000000002</v>
+        <v>19.949999999999996</v>
       </c>
       <c r="I14" s="17">
         <f t="shared" si="1"/>
-        <v>20.700000000000003</v>
+        <v>17.099999999999994</v>
       </c>
       <c r="J14" s="18">
         <f t="shared" si="1"/>
-        <v>17.250000000000004</v>
+        <v>14.249999999999995</v>
       </c>
       <c r="K14" s="17">
         <f t="shared" si="1"/>
-        <v>13.800000000000004</v>
+        <v>11.399999999999995</v>
       </c>
       <c r="L14" s="17">
         <f t="shared" si="1"/>
-        <v>10.350000000000005</v>
+        <v>8.5499999999999954</v>
       </c>
       <c r="M14" s="17">
         <f t="shared" si="1"/>
-        <v>6.9000000000000048</v>
+        <v>5.6999999999999957</v>
       </c>
       <c r="N14" s="17">
         <f t="shared" si="1"/>
-        <v>3.4500000000000046</v>
+        <v>2.8499999999999956</v>
       </c>
       <c r="O14" s="18">
         <f t="shared" si="1"/>
-        <v>4.4408920985006262E-15</v>
+        <v>-4.4408920985006262E-15</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
@@ -8358,47 +8374,47 @@
       <c r="D15" s="33"/>
       <c r="E15" s="10">
         <f>SUM(E4:E13)</f>
-        <v>34.5</v>
+        <v>28.5</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" ref="F15:O15" si="2">E15-(SUM(F4:F13))</f>
-        <v>33.5</v>
+        <v>27.5</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>16.5</v>
       </c>
       <c r="I15" s="6">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>16.5</v>
       </c>
       <c r="J15" s="21">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>11</v>
       </c>
       <c r="K15" s="6">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>9.5</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>7.5</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>7.5</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>7.5</v>
       </c>
       <c r="O15" s="7">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>5.5</v>
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="2"/>
@@ -8454,12 +8470,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9288,14 +9304,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:Q2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>